<commit_message>
Update Import Data Utama
</commit_message>
<xml_diff>
--- a/excel/format-data-utama-siswa.xlsx
+++ b/excel/format-data-utama-siswa.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8490"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <author>Iqbal Revvin</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -144,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -249,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -305,7 +305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -361,7 +361,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -422,12 +422,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>JENIS KELAMIN</t>
-  </si>
-  <si>
-    <t>IMPORT DATA UTAMA SISWA</t>
   </si>
   <si>
     <t>ID SEKOLAH</t>
@@ -469,12 +466,6 @@
     <t>LINK FACEBOOK</t>
   </si>
   <si>
-    <t>INFORMASI KELAHIRAN</t>
-  </si>
-  <si>
-    <t>KOTAK PESERTA DIDIK</t>
-  </si>
-  <si>
     <t>0015801294</t>
   </si>
   <si>
@@ -504,8 +495,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="0000"/>
-    <numFmt numFmtId="173" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="0000"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -537,7 +528,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -550,14 +541,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -580,6 +565,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -595,7 +593,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -604,20 +602,20 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -923,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1203"/>
+  <dimension ref="A1:R1201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,138 +947,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>0</v>
+      <c r="I1" s="8" t="s">
+        <v>8</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="J1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>3205402108010000</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2017</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2">
+        <v>171810309</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="8" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3">
-        <v>3205402108010000</v>
-      </c>
-      <c r="C4" s="4">
-        <v>2017</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="H2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2">
-        <v>171810309</v>
+      <c r="I2" s="7">
+        <v>37063</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="K2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="7">
-        <v>37063</v>
+      <c r="M2" s="5" t="s">
+        <v>20</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>21</v>
+      <c r="N2" s="5" t="s">
+        <v>20</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>22</v>
+      <c r="O2" s="5" t="s">
+        <v>20</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -1089,14 +1087,14 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="6"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="7"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="6"/>
+      <c r="K5" s="11"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1116,7 +1114,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="7"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="6"/>
+      <c r="K6" s="11"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1136,7 +1134,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="7"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="6"/>
+      <c r="K7" s="11"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1156,7 +1154,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="7"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="6"/>
+      <c r="K8" s="11"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1176,7 +1174,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="7"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="6"/>
+      <c r="K9" s="11"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1196,7 +1194,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="7"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="6"/>
+      <c r="K10" s="11"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1216,7 +1214,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="7"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="6"/>
+      <c r="K11" s="11"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1236,7 +1234,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="7"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="6"/>
+      <c r="K12" s="11"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1256,7 +1254,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="7"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="6"/>
+      <c r="K13" s="11"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1276,7 +1274,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="7"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="6"/>
+      <c r="K14" s="11"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1296,7 +1294,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="7"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="6"/>
+      <c r="K15" s="11"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1316,7 +1314,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="7"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="6"/>
+      <c r="K16" s="11"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -1336,7 +1334,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="7"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="6"/>
+      <c r="K17" s="11"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1356,7 +1354,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="7"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="6"/>
+      <c r="K18" s="11"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -1376,7 +1374,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="7"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="6"/>
+      <c r="K19" s="11"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -1396,7 +1394,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="7"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="6"/>
+      <c r="K20" s="11"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -1416,7 +1414,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="7"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="6"/>
+      <c r="K21" s="11"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1436,7 +1434,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="7"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="6"/>
+      <c r="K22" s="11"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1456,7 +1454,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="7"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="6"/>
+      <c r="K23" s="11"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1476,7 +1474,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="7"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="6"/>
+      <c r="K24" s="11"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -1496,7 +1494,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="7"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="6"/>
+      <c r="K25" s="11"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1516,7 +1514,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="7"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="6"/>
+      <c r="K26" s="11"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1529,14 +1527,14 @@
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="5"/>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="7"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="6"/>
+      <c r="K27" s="11"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -1549,14 +1547,14 @@
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="5"/>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="7"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
+      <c r="K28" s="11"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -1576,7 +1574,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="7"/>
       <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+      <c r="K29" s="11"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -1596,7 +1594,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="7"/>
       <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+      <c r="K30" s="11"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -1616,7 +1614,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="7"/>
       <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="K31" s="11"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -1636,7 +1634,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="7"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+      <c r="K32" s="11"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -1656,7 +1654,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="7"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
+      <c r="K33" s="11"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -1676,7 +1674,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="7"/>
       <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
+      <c r="K34" s="11"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -1696,7 +1694,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="7"/>
       <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
+      <c r="K35" s="11"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -1716,7 +1714,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="7"/>
       <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
+      <c r="K36" s="11"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -1736,7 +1734,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="7"/>
       <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
+      <c r="K37" s="11"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -1756,7 +1754,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="7"/>
       <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
+      <c r="K38" s="11"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -1776,7 +1774,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="7"/>
       <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
+      <c r="K39" s="11"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -1796,7 +1794,7 @@
       <c r="H40" s="2"/>
       <c r="I40" s="7"/>
       <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
+      <c r="K40" s="11"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -1816,7 +1814,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="7"/>
       <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
+      <c r="K41" s="11"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -1836,7 +1834,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="7"/>
       <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
+      <c r="K42" s="11"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -1856,7 +1854,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="7"/>
       <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
+      <c r="K43" s="11"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -1876,7 +1874,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="7"/>
       <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
+      <c r="K44" s="11"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -1896,7 +1894,7 @@
       <c r="H45" s="2"/>
       <c r="I45" s="7"/>
       <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
+      <c r="K45" s="11"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -1916,7 +1914,7 @@
       <c r="H46" s="2"/>
       <c r="I46" s="7"/>
       <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
+      <c r="K46" s="11"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -1936,7 +1934,7 @@
       <c r="H47" s="2"/>
       <c r="I47" s="7"/>
       <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
+      <c r="K47" s="11"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -1956,7 +1954,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="7"/>
       <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
+      <c r="K48" s="11"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -1976,7 +1974,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="7"/>
       <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
+      <c r="K49" s="11"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -1996,7 +1994,7 @@
       <c r="H50" s="2"/>
       <c r="I50" s="7"/>
       <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
+      <c r="K50" s="11"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -2016,7 +2014,7 @@
       <c r="H51" s="2"/>
       <c r="I51" s="7"/>
       <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
+      <c r="K51" s="11"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -2036,7 +2034,7 @@
       <c r="H52" s="2"/>
       <c r="I52" s="7"/>
       <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
+      <c r="K52" s="11"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -2056,7 +2054,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="7"/>
       <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
+      <c r="K53" s="11"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -2076,7 +2074,7 @@
       <c r="H54" s="2"/>
       <c r="I54" s="7"/>
       <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
+      <c r="K54" s="11"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -2096,7 +2094,7 @@
       <c r="H55" s="2"/>
       <c r="I55" s="7"/>
       <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
+      <c r="K55" s="11"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -2116,7 +2114,7 @@
       <c r="H56" s="2"/>
       <c r="I56" s="7"/>
       <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
+      <c r="K56" s="11"/>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -2136,7 +2134,7 @@
       <c r="H57" s="2"/>
       <c r="I57" s="7"/>
       <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
+      <c r="K57" s="11"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -2156,7 +2154,7 @@
       <c r="H58" s="2"/>
       <c r="I58" s="7"/>
       <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
+      <c r="K58" s="11"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -2176,7 +2174,7 @@
       <c r="H59" s="2"/>
       <c r="I59" s="7"/>
       <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
+      <c r="K59" s="11"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -2196,7 +2194,7 @@
       <c r="H60" s="2"/>
       <c r="I60" s="7"/>
       <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
+      <c r="K60" s="11"/>
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
@@ -2216,7 +2214,7 @@
       <c r="H61" s="2"/>
       <c r="I61" s="7"/>
       <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
+      <c r="K61" s="11"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -2236,7 +2234,7 @@
       <c r="H62" s="2"/>
       <c r="I62" s="7"/>
       <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
+      <c r="K62" s="11"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -2256,7 +2254,7 @@
       <c r="H63" s="2"/>
       <c r="I63" s="7"/>
       <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
+      <c r="K63" s="11"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -2276,7 +2274,7 @@
       <c r="H64" s="2"/>
       <c r="I64" s="7"/>
       <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
+      <c r="K64" s="11"/>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
@@ -2296,7 +2294,7 @@
       <c r="H65" s="2"/>
       <c r="I65" s="7"/>
       <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
+      <c r="K65" s="11"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -2316,7 +2314,7 @@
       <c r="H66" s="2"/>
       <c r="I66" s="7"/>
       <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
+      <c r="K66" s="11"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -2336,7 +2334,7 @@
       <c r="H67" s="2"/>
       <c r="I67" s="7"/>
       <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
+      <c r="K67" s="11"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -2356,7 +2354,7 @@
       <c r="H68" s="2"/>
       <c r="I68" s="7"/>
       <c r="J68" s="2"/>
-      <c r="K68" s="2"/>
+      <c r="K68" s="11"/>
       <c r="L68" s="2"/>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -2376,7 +2374,7 @@
       <c r="H69" s="2"/>
       <c r="I69" s="7"/>
       <c r="J69" s="2"/>
-      <c r="K69" s="2"/>
+      <c r="K69" s="11"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -2396,7 +2394,7 @@
       <c r="H70" s="2"/>
       <c r="I70" s="7"/>
       <c r="J70" s="2"/>
-      <c r="K70" s="2"/>
+      <c r="K70" s="11"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -2416,7 +2414,7 @@
       <c r="H71" s="2"/>
       <c r="I71" s="7"/>
       <c r="J71" s="2"/>
-      <c r="K71" s="2"/>
+      <c r="K71" s="11"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -2436,7 +2434,7 @@
       <c r="H72" s="2"/>
       <c r="I72" s="7"/>
       <c r="J72" s="2"/>
-      <c r="K72" s="2"/>
+      <c r="K72" s="11"/>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
@@ -2456,7 +2454,7 @@
       <c r="H73" s="2"/>
       <c r="I73" s="7"/>
       <c r="J73" s="2"/>
-      <c r="K73" s="2"/>
+      <c r="K73" s="11"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -2476,7 +2474,7 @@
       <c r="H74" s="2"/>
       <c r="I74" s="7"/>
       <c r="J74" s="2"/>
-      <c r="K74" s="2"/>
+      <c r="K74" s="11"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -2496,7 +2494,7 @@
       <c r="H75" s="2"/>
       <c r="I75" s="7"/>
       <c r="J75" s="2"/>
-      <c r="K75" s="2"/>
+      <c r="K75" s="11"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -2516,7 +2514,7 @@
       <c r="H76" s="2"/>
       <c r="I76" s="7"/>
       <c r="J76" s="2"/>
-      <c r="K76" s="2"/>
+      <c r="K76" s="11"/>
       <c r="L76" s="2"/>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
@@ -2536,7 +2534,7 @@
       <c r="H77" s="2"/>
       <c r="I77" s="7"/>
       <c r="J77" s="2"/>
-      <c r="K77" s="2"/>
+      <c r="K77" s="11"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -2556,7 +2554,7 @@
       <c r="H78" s="2"/>
       <c r="I78" s="7"/>
       <c r="J78" s="2"/>
-      <c r="K78" s="2"/>
+      <c r="K78" s="11"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -2576,7 +2574,7 @@
       <c r="H79" s="2"/>
       <c r="I79" s="7"/>
       <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
+      <c r="K79" s="11"/>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -2596,7 +2594,7 @@
       <c r="H80" s="2"/>
       <c r="I80" s="7"/>
       <c r="J80" s="2"/>
-      <c r="K80" s="2"/>
+      <c r="K80" s="11"/>
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
@@ -2616,7 +2614,7 @@
       <c r="H81" s="2"/>
       <c r="I81" s="7"/>
       <c r="J81" s="2"/>
-      <c r="K81" s="2"/>
+      <c r="K81" s="11"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -2636,7 +2634,7 @@
       <c r="H82" s="2"/>
       <c r="I82" s="7"/>
       <c r="J82" s="2"/>
-      <c r="K82" s="2"/>
+      <c r="K82" s="11"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -2656,7 +2654,7 @@
       <c r="H83" s="2"/>
       <c r="I83" s="7"/>
       <c r="J83" s="2"/>
-      <c r="K83" s="2"/>
+      <c r="K83" s="11"/>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -2676,7 +2674,7 @@
       <c r="H84" s="2"/>
       <c r="I84" s="7"/>
       <c r="J84" s="2"/>
-      <c r="K84" s="2"/>
+      <c r="K84" s="11"/>
       <c r="L84" s="2"/>
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
@@ -2696,7 +2694,7 @@
       <c r="H85" s="2"/>
       <c r="I85" s="7"/>
       <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
+      <c r="K85" s="11"/>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
@@ -2716,7 +2714,7 @@
       <c r="H86" s="2"/>
       <c r="I86" s="7"/>
       <c r="J86" s="2"/>
-      <c r="K86" s="2"/>
+      <c r="K86" s="11"/>
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
@@ -2736,7 +2734,7 @@
       <c r="H87" s="2"/>
       <c r="I87" s="7"/>
       <c r="J87" s="2"/>
-      <c r="K87" s="2"/>
+      <c r="K87" s="11"/>
       <c r="L87" s="2"/>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
@@ -2756,7 +2754,7 @@
       <c r="H88" s="2"/>
       <c r="I88" s="7"/>
       <c r="J88" s="2"/>
-      <c r="K88" s="2"/>
+      <c r="K88" s="11"/>
       <c r="L88" s="2"/>
       <c r="M88" s="2"/>
       <c r="N88" s="2"/>
@@ -2776,7 +2774,7 @@
       <c r="H89" s="2"/>
       <c r="I89" s="7"/>
       <c r="J89" s="2"/>
-      <c r="K89" s="2"/>
+      <c r="K89" s="11"/>
       <c r="L89" s="2"/>
       <c r="M89" s="2"/>
       <c r="N89" s="2"/>
@@ -2796,7 +2794,7 @@
       <c r="H90" s="2"/>
       <c r="I90" s="7"/>
       <c r="J90" s="2"/>
-      <c r="K90" s="2"/>
+      <c r="K90" s="11"/>
       <c r="L90" s="2"/>
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
@@ -2816,7 +2814,7 @@
       <c r="H91" s="2"/>
       <c r="I91" s="7"/>
       <c r="J91" s="2"/>
-      <c r="K91" s="2"/>
+      <c r="K91" s="11"/>
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
@@ -2836,7 +2834,7 @@
       <c r="H92" s="2"/>
       <c r="I92" s="7"/>
       <c r="J92" s="2"/>
-      <c r="K92" s="2"/>
+      <c r="K92" s="11"/>
       <c r="L92" s="2"/>
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
@@ -2856,7 +2854,7 @@
       <c r="H93" s="2"/>
       <c r="I93" s="7"/>
       <c r="J93" s="2"/>
-      <c r="K93" s="2"/>
+      <c r="K93" s="11"/>
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
@@ -2876,7 +2874,7 @@
       <c r="H94" s="2"/>
       <c r="I94" s="7"/>
       <c r="J94" s="2"/>
-      <c r="K94" s="2"/>
+      <c r="K94" s="11"/>
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
       <c r="N94" s="2"/>
@@ -2896,7 +2894,7 @@
       <c r="H95" s="2"/>
       <c r="I95" s="7"/>
       <c r="J95" s="2"/>
-      <c r="K95" s="2"/>
+      <c r="K95" s="11"/>
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
@@ -2916,7 +2914,7 @@
       <c r="H96" s="2"/>
       <c r="I96" s="7"/>
       <c r="J96" s="2"/>
-      <c r="K96" s="2"/>
+      <c r="K96" s="11"/>
       <c r="L96" s="2"/>
       <c r="M96" s="2"/>
       <c r="N96" s="2"/>
@@ -2936,7 +2934,7 @@
       <c r="H97" s="2"/>
       <c r="I97" s="7"/>
       <c r="J97" s="2"/>
-      <c r="K97" s="2"/>
+      <c r="K97" s="11"/>
       <c r="L97" s="2"/>
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
@@ -2956,7 +2954,7 @@
       <c r="H98" s="2"/>
       <c r="I98" s="7"/>
       <c r="J98" s="2"/>
-      <c r="K98" s="2"/>
+      <c r="K98" s="11"/>
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
@@ -2976,7 +2974,7 @@
       <c r="H99" s="2"/>
       <c r="I99" s="7"/>
       <c r="J99" s="2"/>
-      <c r="K99" s="2"/>
+      <c r="K99" s="11"/>
       <c r="L99" s="2"/>
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
@@ -2996,7 +2994,7 @@
       <c r="H100" s="2"/>
       <c r="I100" s="7"/>
       <c r="J100" s="2"/>
-      <c r="K100" s="2"/>
+      <c r="K100" s="11"/>
       <c r="L100" s="2"/>
       <c r="M100" s="2"/>
       <c r="N100" s="2"/>
@@ -3016,7 +3014,7 @@
       <c r="H101" s="2"/>
       <c r="I101" s="7"/>
       <c r="J101" s="2"/>
-      <c r="K101" s="2"/>
+      <c r="K101" s="11"/>
       <c r="L101" s="2"/>
       <c r="M101" s="2"/>
       <c r="N101" s="2"/>
@@ -3036,7 +3034,7 @@
       <c r="H102" s="2"/>
       <c r="I102" s="7"/>
       <c r="J102" s="2"/>
-      <c r="K102" s="2"/>
+      <c r="K102" s="11"/>
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
@@ -3056,7 +3054,7 @@
       <c r="H103" s="2"/>
       <c r="I103" s="7"/>
       <c r="J103" s="2"/>
-      <c r="K103" s="2"/>
+      <c r="K103" s="11"/>
       <c r="L103" s="2"/>
       <c r="M103" s="2"/>
       <c r="N103" s="2"/>
@@ -3076,7 +3074,7 @@
       <c r="H104" s="2"/>
       <c r="I104" s="7"/>
       <c r="J104" s="2"/>
-      <c r="K104" s="2"/>
+      <c r="K104" s="11"/>
       <c r="L104" s="2"/>
       <c r="M104" s="2"/>
       <c r="N104" s="2"/>
@@ -3096,7 +3094,7 @@
       <c r="H105" s="2"/>
       <c r="I105" s="7"/>
       <c r="J105" s="2"/>
-      <c r="K105" s="2"/>
+      <c r="K105" s="11"/>
       <c r="L105" s="2"/>
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
@@ -3116,7 +3114,7 @@
       <c r="H106" s="2"/>
       <c r="I106" s="7"/>
       <c r="J106" s="2"/>
-      <c r="K106" s="2"/>
+      <c r="K106" s="11"/>
       <c r="L106" s="2"/>
       <c r="M106" s="2"/>
       <c r="N106" s="2"/>
@@ -3136,7 +3134,7 @@
       <c r="H107" s="2"/>
       <c r="I107" s="7"/>
       <c r="J107" s="2"/>
-      <c r="K107" s="2"/>
+      <c r="K107" s="11"/>
       <c r="L107" s="2"/>
       <c r="M107" s="2"/>
       <c r="N107" s="2"/>
@@ -3156,7 +3154,7 @@
       <c r="H108" s="2"/>
       <c r="I108" s="7"/>
       <c r="J108" s="2"/>
-      <c r="K108" s="2"/>
+      <c r="K108" s="11"/>
       <c r="L108" s="2"/>
       <c r="M108" s="2"/>
       <c r="N108" s="2"/>
@@ -3176,7 +3174,7 @@
       <c r="H109" s="2"/>
       <c r="I109" s="7"/>
       <c r="J109" s="2"/>
-      <c r="K109" s="2"/>
+      <c r="K109" s="11"/>
       <c r="L109" s="2"/>
       <c r="M109" s="2"/>
       <c r="N109" s="2"/>
@@ -3196,7 +3194,7 @@
       <c r="H110" s="2"/>
       <c r="I110" s="7"/>
       <c r="J110" s="2"/>
-      <c r="K110" s="2"/>
+      <c r="K110" s="11"/>
       <c r="L110" s="2"/>
       <c r="M110" s="2"/>
       <c r="N110" s="2"/>
@@ -3216,7 +3214,7 @@
       <c r="H111" s="2"/>
       <c r="I111" s="7"/>
       <c r="J111" s="2"/>
-      <c r="K111" s="2"/>
+      <c r="K111" s="11"/>
       <c r="L111" s="2"/>
       <c r="M111" s="2"/>
       <c r="N111" s="2"/>
@@ -3236,7 +3234,7 @@
       <c r="H112" s="2"/>
       <c r="I112" s="7"/>
       <c r="J112" s="2"/>
-      <c r="K112" s="2"/>
+      <c r="K112" s="11"/>
       <c r="L112" s="2"/>
       <c r="M112" s="2"/>
       <c r="N112" s="2"/>
@@ -3256,7 +3254,7 @@
       <c r="H113" s="2"/>
       <c r="I113" s="7"/>
       <c r="J113" s="2"/>
-      <c r="K113" s="2"/>
+      <c r="K113" s="11"/>
       <c r="L113" s="2"/>
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
@@ -3276,7 +3274,7 @@
       <c r="H114" s="2"/>
       <c r="I114" s="7"/>
       <c r="J114" s="2"/>
-      <c r="K114" s="2"/>
+      <c r="K114" s="11"/>
       <c r="L114" s="2"/>
       <c r="M114" s="2"/>
       <c r="N114" s="2"/>
@@ -3296,7 +3294,7 @@
       <c r="H115" s="2"/>
       <c r="I115" s="7"/>
       <c r="J115" s="2"/>
-      <c r="K115" s="2"/>
+      <c r="K115" s="11"/>
       <c r="L115" s="2"/>
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
@@ -3316,7 +3314,7 @@
       <c r="H116" s="2"/>
       <c r="I116" s="7"/>
       <c r="J116" s="2"/>
-      <c r="K116" s="2"/>
+      <c r="K116" s="11"/>
       <c r="L116" s="2"/>
       <c r="M116" s="2"/>
       <c r="N116" s="2"/>
@@ -3336,7 +3334,7 @@
       <c r="H117" s="2"/>
       <c r="I117" s="7"/>
       <c r="J117" s="2"/>
-      <c r="K117" s="2"/>
+      <c r="K117" s="11"/>
       <c r="L117" s="2"/>
       <c r="M117" s="2"/>
       <c r="N117" s="2"/>
@@ -3356,7 +3354,7 @@
       <c r="H118" s="2"/>
       <c r="I118" s="7"/>
       <c r="J118" s="2"/>
-      <c r="K118" s="2"/>
+      <c r="K118" s="11"/>
       <c r="L118" s="2"/>
       <c r="M118" s="2"/>
       <c r="N118" s="2"/>
@@ -3376,7 +3374,7 @@
       <c r="H119" s="2"/>
       <c r="I119" s="7"/>
       <c r="J119" s="2"/>
-      <c r="K119" s="2"/>
+      <c r="K119" s="11"/>
       <c r="L119" s="2"/>
       <c r="M119" s="2"/>
       <c r="N119" s="2"/>
@@ -3396,7 +3394,7 @@
       <c r="H120" s="2"/>
       <c r="I120" s="7"/>
       <c r="J120" s="2"/>
-      <c r="K120" s="2"/>
+      <c r="K120" s="11"/>
       <c r="L120" s="2"/>
       <c r="M120" s="2"/>
       <c r="N120" s="2"/>
@@ -3416,7 +3414,7 @@
       <c r="H121" s="2"/>
       <c r="I121" s="7"/>
       <c r="J121" s="2"/>
-      <c r="K121" s="2"/>
+      <c r="K121" s="11"/>
       <c r="L121" s="2"/>
       <c r="M121" s="2"/>
       <c r="N121" s="2"/>
@@ -3436,7 +3434,7 @@
       <c r="H122" s="2"/>
       <c r="I122" s="7"/>
       <c r="J122" s="2"/>
-      <c r="K122" s="2"/>
+      <c r="K122" s="11"/>
       <c r="L122" s="2"/>
       <c r="M122" s="2"/>
       <c r="N122" s="2"/>
@@ -3456,7 +3454,7 @@
       <c r="H123" s="2"/>
       <c r="I123" s="7"/>
       <c r="J123" s="2"/>
-      <c r="K123" s="2"/>
+      <c r="K123" s="11"/>
       <c r="L123" s="2"/>
       <c r="M123" s="2"/>
       <c r="N123" s="2"/>
@@ -3476,7 +3474,7 @@
       <c r="H124" s="2"/>
       <c r="I124" s="7"/>
       <c r="J124" s="2"/>
-      <c r="K124" s="2"/>
+      <c r="K124" s="11"/>
       <c r="L124" s="2"/>
       <c r="M124" s="2"/>
       <c r="N124" s="2"/>
@@ -3496,7 +3494,7 @@
       <c r="H125" s="2"/>
       <c r="I125" s="7"/>
       <c r="J125" s="2"/>
-      <c r="K125" s="2"/>
+      <c r="K125" s="11"/>
       <c r="L125" s="2"/>
       <c r="M125" s="2"/>
       <c r="N125" s="2"/>
@@ -3516,7 +3514,7 @@
       <c r="H126" s="2"/>
       <c r="I126" s="7"/>
       <c r="J126" s="2"/>
-      <c r="K126" s="2"/>
+      <c r="K126" s="11"/>
       <c r="L126" s="2"/>
       <c r="M126" s="2"/>
       <c r="N126" s="2"/>
@@ -3536,7 +3534,7 @@
       <c r="H127" s="2"/>
       <c r="I127" s="7"/>
       <c r="J127" s="2"/>
-      <c r="K127" s="2"/>
+      <c r="K127" s="11"/>
       <c r="L127" s="2"/>
       <c r="M127" s="2"/>
       <c r="N127" s="2"/>
@@ -3556,7 +3554,7 @@
       <c r="H128" s="2"/>
       <c r="I128" s="7"/>
       <c r="J128" s="2"/>
-      <c r="K128" s="2"/>
+      <c r="K128" s="11"/>
       <c r="L128" s="2"/>
       <c r="M128" s="2"/>
       <c r="N128" s="2"/>
@@ -3576,7 +3574,7 @@
       <c r="H129" s="2"/>
       <c r="I129" s="7"/>
       <c r="J129" s="2"/>
-      <c r="K129" s="2"/>
+      <c r="K129" s="11"/>
       <c r="L129" s="2"/>
       <c r="M129" s="2"/>
       <c r="N129" s="2"/>
@@ -3596,7 +3594,7 @@
       <c r="H130" s="2"/>
       <c r="I130" s="7"/>
       <c r="J130" s="2"/>
-      <c r="K130" s="2"/>
+      <c r="K130" s="11"/>
       <c r="L130" s="2"/>
       <c r="M130" s="2"/>
       <c r="N130" s="2"/>
@@ -3616,7 +3614,7 @@
       <c r="H131" s="2"/>
       <c r="I131" s="7"/>
       <c r="J131" s="2"/>
-      <c r="K131" s="2"/>
+      <c r="K131" s="11"/>
       <c r="L131" s="2"/>
       <c r="M131" s="2"/>
       <c r="N131" s="2"/>
@@ -3636,7 +3634,7 @@
       <c r="H132" s="2"/>
       <c r="I132" s="7"/>
       <c r="J132" s="2"/>
-      <c r="K132" s="2"/>
+      <c r="K132" s="11"/>
       <c r="L132" s="2"/>
       <c r="M132" s="2"/>
       <c r="N132" s="2"/>
@@ -3656,7 +3654,7 @@
       <c r="H133" s="2"/>
       <c r="I133" s="7"/>
       <c r="J133" s="2"/>
-      <c r="K133" s="2"/>
+      <c r="K133" s="11"/>
       <c r="L133" s="2"/>
       <c r="M133" s="2"/>
       <c r="N133" s="2"/>
@@ -3676,7 +3674,7 @@
       <c r="H134" s="2"/>
       <c r="I134" s="7"/>
       <c r="J134" s="2"/>
-      <c r="K134" s="2"/>
+      <c r="K134" s="11"/>
       <c r="L134" s="2"/>
       <c r="M134" s="2"/>
       <c r="N134" s="2"/>
@@ -3696,7 +3694,7 @@
       <c r="H135" s="2"/>
       <c r="I135" s="7"/>
       <c r="J135" s="2"/>
-      <c r="K135" s="2"/>
+      <c r="K135" s="11"/>
       <c r="L135" s="2"/>
       <c r="M135" s="2"/>
       <c r="N135" s="2"/>
@@ -3716,7 +3714,7 @@
       <c r="H136" s="2"/>
       <c r="I136" s="7"/>
       <c r="J136" s="2"/>
-      <c r="K136" s="2"/>
+      <c r="K136" s="11"/>
       <c r="L136" s="2"/>
       <c r="M136" s="2"/>
       <c r="N136" s="2"/>
@@ -3736,7 +3734,7 @@
       <c r="H137" s="2"/>
       <c r="I137" s="7"/>
       <c r="J137" s="2"/>
-      <c r="K137" s="2"/>
+      <c r="K137" s="11"/>
       <c r="L137" s="2"/>
       <c r="M137" s="2"/>
       <c r="N137" s="2"/>
@@ -3756,7 +3754,7 @@
       <c r="H138" s="2"/>
       <c r="I138" s="7"/>
       <c r="J138" s="2"/>
-      <c r="K138" s="2"/>
+      <c r="K138" s="11"/>
       <c r="L138" s="2"/>
       <c r="M138" s="2"/>
       <c r="N138" s="2"/>
@@ -3776,7 +3774,7 @@
       <c r="H139" s="2"/>
       <c r="I139" s="7"/>
       <c r="J139" s="2"/>
-      <c r="K139" s="2"/>
+      <c r="K139" s="11"/>
       <c r="L139" s="2"/>
       <c r="M139" s="2"/>
       <c r="N139" s="2"/>
@@ -3796,7 +3794,7 @@
       <c r="H140" s="2"/>
       <c r="I140" s="7"/>
       <c r="J140" s="2"/>
-      <c r="K140" s="2"/>
+      <c r="K140" s="11"/>
       <c r="L140" s="2"/>
       <c r="M140" s="2"/>
       <c r="N140" s="2"/>
@@ -3816,7 +3814,7 @@
       <c r="H141" s="2"/>
       <c r="I141" s="7"/>
       <c r="J141" s="2"/>
-      <c r="K141" s="2"/>
+      <c r="K141" s="11"/>
       <c r="L141" s="2"/>
       <c r="M141" s="2"/>
       <c r="N141" s="2"/>
@@ -3836,7 +3834,7 @@
       <c r="H142" s="2"/>
       <c r="I142" s="7"/>
       <c r="J142" s="2"/>
-      <c r="K142" s="2"/>
+      <c r="K142" s="11"/>
       <c r="L142" s="2"/>
       <c r="M142" s="2"/>
       <c r="N142" s="2"/>
@@ -3856,7 +3854,7 @@
       <c r="H143" s="2"/>
       <c r="I143" s="7"/>
       <c r="J143" s="2"/>
-      <c r="K143" s="2"/>
+      <c r="K143" s="11"/>
       <c r="L143" s="2"/>
       <c r="M143" s="2"/>
       <c r="N143" s="2"/>
@@ -3876,7 +3874,7 @@
       <c r="H144" s="2"/>
       <c r="I144" s="7"/>
       <c r="J144" s="2"/>
-      <c r="K144" s="2"/>
+      <c r="K144" s="11"/>
       <c r="L144" s="2"/>
       <c r="M144" s="2"/>
       <c r="N144" s="2"/>
@@ -3896,7 +3894,7 @@
       <c r="H145" s="2"/>
       <c r="I145" s="7"/>
       <c r="J145" s="2"/>
-      <c r="K145" s="2"/>
+      <c r="K145" s="11"/>
       <c r="L145" s="2"/>
       <c r="M145" s="2"/>
       <c r="N145" s="2"/>
@@ -3916,7 +3914,7 @@
       <c r="H146" s="2"/>
       <c r="I146" s="7"/>
       <c r="J146" s="2"/>
-      <c r="K146" s="2"/>
+      <c r="K146" s="11"/>
       <c r="L146" s="2"/>
       <c r="M146" s="2"/>
       <c r="N146" s="2"/>
@@ -3936,7 +3934,7 @@
       <c r="H147" s="2"/>
       <c r="I147" s="7"/>
       <c r="J147" s="2"/>
-      <c r="K147" s="2"/>
+      <c r="K147" s="11"/>
       <c r="L147" s="2"/>
       <c r="M147" s="2"/>
       <c r="N147" s="2"/>
@@ -3956,7 +3954,7 @@
       <c r="H148" s="2"/>
       <c r="I148" s="7"/>
       <c r="J148" s="2"/>
-      <c r="K148" s="2"/>
+      <c r="K148" s="11"/>
       <c r="L148" s="2"/>
       <c r="M148" s="2"/>
       <c r="N148" s="2"/>
@@ -3976,7 +3974,7 @@
       <c r="H149" s="2"/>
       <c r="I149" s="7"/>
       <c r="J149" s="2"/>
-      <c r="K149" s="2"/>
+      <c r="K149" s="11"/>
       <c r="L149" s="2"/>
       <c r="M149" s="2"/>
       <c r="N149" s="2"/>
@@ -3996,7 +3994,7 @@
       <c r="H150" s="2"/>
       <c r="I150" s="7"/>
       <c r="J150" s="2"/>
-      <c r="K150" s="2"/>
+      <c r="K150" s="11"/>
       <c r="L150" s="2"/>
       <c r="M150" s="2"/>
       <c r="N150" s="2"/>
@@ -4016,7 +4014,7 @@
       <c r="H151" s="2"/>
       <c r="I151" s="7"/>
       <c r="J151" s="2"/>
-      <c r="K151" s="2"/>
+      <c r="K151" s="11"/>
       <c r="L151" s="2"/>
       <c r="M151" s="2"/>
       <c r="N151" s="2"/>
@@ -4036,7 +4034,7 @@
       <c r="H152" s="2"/>
       <c r="I152" s="7"/>
       <c r="J152" s="2"/>
-      <c r="K152" s="2"/>
+      <c r="K152" s="11"/>
       <c r="L152" s="2"/>
       <c r="M152" s="2"/>
       <c r="N152" s="2"/>
@@ -4056,7 +4054,7 @@
       <c r="H153" s="2"/>
       <c r="I153" s="7"/>
       <c r="J153" s="2"/>
-      <c r="K153" s="2"/>
+      <c r="K153" s="11"/>
       <c r="L153" s="2"/>
       <c r="M153" s="2"/>
       <c r="N153" s="2"/>
@@ -4076,7 +4074,7 @@
       <c r="H154" s="2"/>
       <c r="I154" s="7"/>
       <c r="J154" s="2"/>
-      <c r="K154" s="2"/>
+      <c r="K154" s="11"/>
       <c r="L154" s="2"/>
       <c r="M154" s="2"/>
       <c r="N154" s="2"/>
@@ -4096,7 +4094,7 @@
       <c r="H155" s="2"/>
       <c r="I155" s="7"/>
       <c r="J155" s="2"/>
-      <c r="K155" s="2"/>
+      <c r="K155" s="11"/>
       <c r="L155" s="2"/>
       <c r="M155" s="2"/>
       <c r="N155" s="2"/>
@@ -4116,7 +4114,7 @@
       <c r="H156" s="2"/>
       <c r="I156" s="7"/>
       <c r="J156" s="2"/>
-      <c r="K156" s="2"/>
+      <c r="K156" s="11"/>
       <c r="L156" s="2"/>
       <c r="M156" s="2"/>
       <c r="N156" s="2"/>
@@ -4136,7 +4134,7 @@
       <c r="H157" s="2"/>
       <c r="I157" s="7"/>
       <c r="J157" s="2"/>
-      <c r="K157" s="2"/>
+      <c r="K157" s="11"/>
       <c r="L157" s="2"/>
       <c r="M157" s="2"/>
       <c r="N157" s="2"/>
@@ -4156,7 +4154,7 @@
       <c r="H158" s="2"/>
       <c r="I158" s="7"/>
       <c r="J158" s="2"/>
-      <c r="K158" s="2"/>
+      <c r="K158" s="11"/>
       <c r="L158" s="2"/>
       <c r="M158" s="2"/>
       <c r="N158" s="2"/>
@@ -4176,7 +4174,7 @@
       <c r="H159" s="2"/>
       <c r="I159" s="7"/>
       <c r="J159" s="2"/>
-      <c r="K159" s="2"/>
+      <c r="K159" s="11"/>
       <c r="L159" s="2"/>
       <c r="M159" s="2"/>
       <c r="N159" s="2"/>
@@ -4196,7 +4194,7 @@
       <c r="H160" s="2"/>
       <c r="I160" s="7"/>
       <c r="J160" s="2"/>
-      <c r="K160" s="2"/>
+      <c r="K160" s="11"/>
       <c r="L160" s="2"/>
       <c r="M160" s="2"/>
       <c r="N160" s="2"/>
@@ -4216,7 +4214,7 @@
       <c r="H161" s="2"/>
       <c r="I161" s="7"/>
       <c r="J161" s="2"/>
-      <c r="K161" s="2"/>
+      <c r="K161" s="11"/>
       <c r="L161" s="2"/>
       <c r="M161" s="2"/>
       <c r="N161" s="2"/>
@@ -4236,7 +4234,7 @@
       <c r="H162" s="2"/>
       <c r="I162" s="7"/>
       <c r="J162" s="2"/>
-      <c r="K162" s="2"/>
+      <c r="K162" s="11"/>
       <c r="L162" s="2"/>
       <c r="M162" s="2"/>
       <c r="N162" s="2"/>
@@ -4256,7 +4254,7 @@
       <c r="H163" s="2"/>
       <c r="I163" s="7"/>
       <c r="J163" s="2"/>
-      <c r="K163" s="2"/>
+      <c r="K163" s="11"/>
       <c r="L163" s="2"/>
       <c r="M163" s="2"/>
       <c r="N163" s="2"/>
@@ -4276,7 +4274,7 @@
       <c r="H164" s="2"/>
       <c r="I164" s="7"/>
       <c r="J164" s="2"/>
-      <c r="K164" s="2"/>
+      <c r="K164" s="11"/>
       <c r="L164" s="2"/>
       <c r="M164" s="2"/>
       <c r="N164" s="2"/>
@@ -4296,7 +4294,7 @@
       <c r="H165" s="2"/>
       <c r="I165" s="7"/>
       <c r="J165" s="2"/>
-      <c r="K165" s="2"/>
+      <c r="K165" s="11"/>
       <c r="L165" s="2"/>
       <c r="M165" s="2"/>
       <c r="N165" s="2"/>
@@ -4316,7 +4314,7 @@
       <c r="H166" s="2"/>
       <c r="I166" s="7"/>
       <c r="J166" s="2"/>
-      <c r="K166" s="2"/>
+      <c r="K166" s="11"/>
       <c r="L166" s="2"/>
       <c r="M166" s="2"/>
       <c r="N166" s="2"/>
@@ -4336,7 +4334,7 @@
       <c r="H167" s="2"/>
       <c r="I167" s="7"/>
       <c r="J167" s="2"/>
-      <c r="K167" s="2"/>
+      <c r="K167" s="11"/>
       <c r="L167" s="2"/>
       <c r="M167" s="2"/>
       <c r="N167" s="2"/>
@@ -4356,7 +4354,7 @@
       <c r="H168" s="2"/>
       <c r="I168" s="7"/>
       <c r="J168" s="2"/>
-      <c r="K168" s="2"/>
+      <c r="K168" s="11"/>
       <c r="L168" s="2"/>
       <c r="M168" s="2"/>
       <c r="N168" s="2"/>
@@ -4376,7 +4374,7 @@
       <c r="H169" s="2"/>
       <c r="I169" s="7"/>
       <c r="J169" s="2"/>
-      <c r="K169" s="2"/>
+      <c r="K169" s="11"/>
       <c r="L169" s="2"/>
       <c r="M169" s="2"/>
       <c r="N169" s="2"/>
@@ -4396,7 +4394,7 @@
       <c r="H170" s="2"/>
       <c r="I170" s="7"/>
       <c r="J170" s="2"/>
-      <c r="K170" s="2"/>
+      <c r="K170" s="11"/>
       <c r="L170" s="2"/>
       <c r="M170" s="2"/>
       <c r="N170" s="2"/>
@@ -4416,7 +4414,7 @@
       <c r="H171" s="2"/>
       <c r="I171" s="7"/>
       <c r="J171" s="2"/>
-      <c r="K171" s="2"/>
+      <c r="K171" s="11"/>
       <c r="L171" s="2"/>
       <c r="M171" s="2"/>
       <c r="N171" s="2"/>
@@ -4436,7 +4434,7 @@
       <c r="H172" s="2"/>
       <c r="I172" s="7"/>
       <c r="J172" s="2"/>
-      <c r="K172" s="2"/>
+      <c r="K172" s="11"/>
       <c r="L172" s="2"/>
       <c r="M172" s="2"/>
       <c r="N172" s="2"/>
@@ -4456,7 +4454,7 @@
       <c r="H173" s="2"/>
       <c r="I173" s="7"/>
       <c r="J173" s="2"/>
-      <c r="K173" s="2"/>
+      <c r="K173" s="11"/>
       <c r="L173" s="2"/>
       <c r="M173" s="2"/>
       <c r="N173" s="2"/>
@@ -4476,7 +4474,7 @@
       <c r="H174" s="2"/>
       <c r="I174" s="7"/>
       <c r="J174" s="2"/>
-      <c r="K174" s="2"/>
+      <c r="K174" s="11"/>
       <c r="L174" s="2"/>
       <c r="M174" s="2"/>
       <c r="N174" s="2"/>
@@ -4496,7 +4494,7 @@
       <c r="H175" s="2"/>
       <c r="I175" s="7"/>
       <c r="J175" s="2"/>
-      <c r="K175" s="2"/>
+      <c r="K175" s="11"/>
       <c r="L175" s="2"/>
       <c r="M175" s="2"/>
       <c r="N175" s="2"/>
@@ -4516,7 +4514,7 @@
       <c r="H176" s="2"/>
       <c r="I176" s="7"/>
       <c r="J176" s="2"/>
-      <c r="K176" s="2"/>
+      <c r="K176" s="11"/>
       <c r="L176" s="2"/>
       <c r="M176" s="2"/>
       <c r="N176" s="2"/>
@@ -4536,7 +4534,7 @@
       <c r="H177" s="2"/>
       <c r="I177" s="7"/>
       <c r="J177" s="2"/>
-      <c r="K177" s="2"/>
+      <c r="K177" s="11"/>
       <c r="L177" s="2"/>
       <c r="M177" s="2"/>
       <c r="N177" s="2"/>
@@ -4556,7 +4554,7 @@
       <c r="H178" s="2"/>
       <c r="I178" s="7"/>
       <c r="J178" s="2"/>
-      <c r="K178" s="2"/>
+      <c r="K178" s="11"/>
       <c r="L178" s="2"/>
       <c r="M178" s="2"/>
       <c r="N178" s="2"/>
@@ -4576,7 +4574,7 @@
       <c r="H179" s="2"/>
       <c r="I179" s="7"/>
       <c r="J179" s="2"/>
-      <c r="K179" s="2"/>
+      <c r="K179" s="11"/>
       <c r="L179" s="2"/>
       <c r="M179" s="2"/>
       <c r="N179" s="2"/>
@@ -4596,7 +4594,7 @@
       <c r="H180" s="2"/>
       <c r="I180" s="7"/>
       <c r="J180" s="2"/>
-      <c r="K180" s="2"/>
+      <c r="K180" s="11"/>
       <c r="L180" s="2"/>
       <c r="M180" s="2"/>
       <c r="N180" s="2"/>
@@ -4616,7 +4614,7 @@
       <c r="H181" s="2"/>
       <c r="I181" s="7"/>
       <c r="J181" s="2"/>
-      <c r="K181" s="2"/>
+      <c r="K181" s="11"/>
       <c r="L181" s="2"/>
       <c r="M181" s="2"/>
       <c r="N181" s="2"/>
@@ -4636,7 +4634,7 @@
       <c r="H182" s="2"/>
       <c r="I182" s="7"/>
       <c r="J182" s="2"/>
-      <c r="K182" s="2"/>
+      <c r="K182" s="11"/>
       <c r="L182" s="2"/>
       <c r="M182" s="2"/>
       <c r="N182" s="2"/>
@@ -4656,7 +4654,7 @@
       <c r="H183" s="2"/>
       <c r="I183" s="7"/>
       <c r="J183" s="2"/>
-      <c r="K183" s="2"/>
+      <c r="K183" s="11"/>
       <c r="L183" s="2"/>
       <c r="M183" s="2"/>
       <c r="N183" s="2"/>
@@ -4676,7 +4674,7 @@
       <c r="H184" s="2"/>
       <c r="I184" s="7"/>
       <c r="J184" s="2"/>
-      <c r="K184" s="2"/>
+      <c r="K184" s="11"/>
       <c r="L184" s="2"/>
       <c r="M184" s="2"/>
       <c r="N184" s="2"/>
@@ -4696,7 +4694,7 @@
       <c r="H185" s="2"/>
       <c r="I185" s="7"/>
       <c r="J185" s="2"/>
-      <c r="K185" s="2"/>
+      <c r="K185" s="11"/>
       <c r="L185" s="2"/>
       <c r="M185" s="2"/>
       <c r="N185" s="2"/>
@@ -4716,7 +4714,7 @@
       <c r="H186" s="2"/>
       <c r="I186" s="7"/>
       <c r="J186" s="2"/>
-      <c r="K186" s="2"/>
+      <c r="K186" s="11"/>
       <c r="L186" s="2"/>
       <c r="M186" s="2"/>
       <c r="N186" s="2"/>
@@ -4736,7 +4734,7 @@
       <c r="H187" s="2"/>
       <c r="I187" s="7"/>
       <c r="J187" s="2"/>
-      <c r="K187" s="2"/>
+      <c r="K187" s="11"/>
       <c r="L187" s="2"/>
       <c r="M187" s="2"/>
       <c r="N187" s="2"/>
@@ -4756,7 +4754,7 @@
       <c r="H188" s="2"/>
       <c r="I188" s="7"/>
       <c r="J188" s="2"/>
-      <c r="K188" s="2"/>
+      <c r="K188" s="11"/>
       <c r="L188" s="2"/>
       <c r="M188" s="2"/>
       <c r="N188" s="2"/>
@@ -4776,7 +4774,7 @@
       <c r="H189" s="2"/>
       <c r="I189" s="7"/>
       <c r="J189" s="2"/>
-      <c r="K189" s="2"/>
+      <c r="K189" s="11"/>
       <c r="L189" s="2"/>
       <c r="M189" s="2"/>
       <c r="N189" s="2"/>
@@ -4796,7 +4794,7 @@
       <c r="H190" s="2"/>
       <c r="I190" s="7"/>
       <c r="J190" s="2"/>
-      <c r="K190" s="2"/>
+      <c r="K190" s="11"/>
       <c r="L190" s="2"/>
       <c r="M190" s="2"/>
       <c r="N190" s="2"/>
@@ -4816,7 +4814,7 @@
       <c r="H191" s="2"/>
       <c r="I191" s="7"/>
       <c r="J191" s="2"/>
-      <c r="K191" s="2"/>
+      <c r="K191" s="11"/>
       <c r="L191" s="2"/>
       <c r="M191" s="2"/>
       <c r="N191" s="2"/>
@@ -4836,7 +4834,7 @@
       <c r="H192" s="2"/>
       <c r="I192" s="7"/>
       <c r="J192" s="2"/>
-      <c r="K192" s="2"/>
+      <c r="K192" s="11"/>
       <c r="L192" s="2"/>
       <c r="M192" s="2"/>
       <c r="N192" s="2"/>
@@ -4856,7 +4854,7 @@
       <c r="H193" s="2"/>
       <c r="I193" s="7"/>
       <c r="J193" s="2"/>
-      <c r="K193" s="2"/>
+      <c r="K193" s="11"/>
       <c r="L193" s="2"/>
       <c r="M193" s="2"/>
       <c r="N193" s="2"/>
@@ -4876,7 +4874,7 @@
       <c r="H194" s="2"/>
       <c r="I194" s="7"/>
       <c r="J194" s="2"/>
-      <c r="K194" s="2"/>
+      <c r="K194" s="11"/>
       <c r="L194" s="2"/>
       <c r="M194" s="2"/>
       <c r="N194" s="2"/>
@@ -4896,7 +4894,7 @@
       <c r="H195" s="2"/>
       <c r="I195" s="7"/>
       <c r="J195" s="2"/>
-      <c r="K195" s="2"/>
+      <c r="K195" s="11"/>
       <c r="L195" s="2"/>
       <c r="M195" s="2"/>
       <c r="N195" s="2"/>
@@ -4916,7 +4914,7 @@
       <c r="H196" s="2"/>
       <c r="I196" s="7"/>
       <c r="J196" s="2"/>
-      <c r="K196" s="2"/>
+      <c r="K196" s="11"/>
       <c r="L196" s="2"/>
       <c r="M196" s="2"/>
       <c r="N196" s="2"/>
@@ -4936,7 +4934,7 @@
       <c r="H197" s="2"/>
       <c r="I197" s="7"/>
       <c r="J197" s="2"/>
-      <c r="K197" s="2"/>
+      <c r="K197" s="11"/>
       <c r="L197" s="2"/>
       <c r="M197" s="2"/>
       <c r="N197" s="2"/>
@@ -4956,7 +4954,7 @@
       <c r="H198" s="2"/>
       <c r="I198" s="7"/>
       <c r="J198" s="2"/>
-      <c r="K198" s="2"/>
+      <c r="K198" s="11"/>
       <c r="L198" s="2"/>
       <c r="M198" s="2"/>
       <c r="N198" s="2"/>
@@ -4976,7 +4974,7 @@
       <c r="H199" s="2"/>
       <c r="I199" s="7"/>
       <c r="J199" s="2"/>
-      <c r="K199" s="2"/>
+      <c r="K199" s="11"/>
       <c r="L199" s="2"/>
       <c r="M199" s="2"/>
       <c r="N199" s="2"/>
@@ -4996,7 +4994,7 @@
       <c r="H200" s="2"/>
       <c r="I200" s="7"/>
       <c r="J200" s="2"/>
-      <c r="K200" s="2"/>
+      <c r="K200" s="11"/>
       <c r="L200" s="2"/>
       <c r="M200" s="2"/>
       <c r="N200" s="2"/>
@@ -5016,7 +5014,7 @@
       <c r="H201" s="2"/>
       <c r="I201" s="7"/>
       <c r="J201" s="2"/>
-      <c r="K201" s="2"/>
+      <c r="K201" s="11"/>
       <c r="L201" s="2"/>
       <c r="M201" s="2"/>
       <c r="N201" s="2"/>
@@ -5036,7 +5034,7 @@
       <c r="H202" s="2"/>
       <c r="I202" s="7"/>
       <c r="J202" s="2"/>
-      <c r="K202" s="2"/>
+      <c r="K202" s="11"/>
       <c r="L202" s="2"/>
       <c r="M202" s="2"/>
       <c r="N202" s="2"/>
@@ -5056,7 +5054,7 @@
       <c r="H203" s="2"/>
       <c r="I203" s="7"/>
       <c r="J203" s="2"/>
-      <c r="K203" s="2"/>
+      <c r="K203" s="11"/>
       <c r="L203" s="2"/>
       <c r="M203" s="2"/>
       <c r="N203" s="2"/>
@@ -5076,7 +5074,7 @@
       <c r="H204" s="2"/>
       <c r="I204" s="7"/>
       <c r="J204" s="2"/>
-      <c r="K204" s="2"/>
+      <c r="K204" s="11"/>
       <c r="L204" s="2"/>
       <c r="M204" s="2"/>
       <c r="N204" s="2"/>
@@ -5096,7 +5094,7 @@
       <c r="H205" s="2"/>
       <c r="I205" s="7"/>
       <c r="J205" s="2"/>
-      <c r="K205" s="2"/>
+      <c r="K205" s="11"/>
       <c r="L205" s="2"/>
       <c r="M205" s="2"/>
       <c r="N205" s="2"/>
@@ -5116,7 +5114,7 @@
       <c r="H206" s="2"/>
       <c r="I206" s="7"/>
       <c r="J206" s="2"/>
-      <c r="K206" s="2"/>
+      <c r="K206" s="11"/>
       <c r="L206" s="2"/>
       <c r="M206" s="2"/>
       <c r="N206" s="2"/>
@@ -5136,7 +5134,7 @@
       <c r="H207" s="2"/>
       <c r="I207" s="7"/>
       <c r="J207" s="2"/>
-      <c r="K207" s="2"/>
+      <c r="K207" s="11"/>
       <c r="L207" s="2"/>
       <c r="M207" s="2"/>
       <c r="N207" s="2"/>
@@ -5156,7 +5154,7 @@
       <c r="H208" s="2"/>
       <c r="I208" s="7"/>
       <c r="J208" s="2"/>
-      <c r="K208" s="2"/>
+      <c r="K208" s="11"/>
       <c r="L208" s="2"/>
       <c r="M208" s="2"/>
       <c r="N208" s="2"/>
@@ -5176,7 +5174,7 @@
       <c r="H209" s="2"/>
       <c r="I209" s="7"/>
       <c r="J209" s="2"/>
-      <c r="K209" s="2"/>
+      <c r="K209" s="11"/>
       <c r="L209" s="2"/>
       <c r="M209" s="2"/>
       <c r="N209" s="2"/>
@@ -5196,7 +5194,7 @@
       <c r="H210" s="2"/>
       <c r="I210" s="7"/>
       <c r="J210" s="2"/>
-      <c r="K210" s="2"/>
+      <c r="K210" s="11"/>
       <c r="L210" s="2"/>
       <c r="M210" s="2"/>
       <c r="N210" s="2"/>
@@ -5216,7 +5214,7 @@
       <c r="H211" s="2"/>
       <c r="I211" s="7"/>
       <c r="J211" s="2"/>
-      <c r="K211" s="2"/>
+      <c r="K211" s="11"/>
       <c r="L211" s="2"/>
       <c r="M211" s="2"/>
       <c r="N211" s="2"/>
@@ -5236,7 +5234,7 @@
       <c r="H212" s="2"/>
       <c r="I212" s="7"/>
       <c r="J212" s="2"/>
-      <c r="K212" s="2"/>
+      <c r="K212" s="11"/>
       <c r="L212" s="2"/>
       <c r="M212" s="2"/>
       <c r="N212" s="2"/>
@@ -5256,7 +5254,7 @@
       <c r="H213" s="2"/>
       <c r="I213" s="7"/>
       <c r="J213" s="2"/>
-      <c r="K213" s="2"/>
+      <c r="K213" s="11"/>
       <c r="L213" s="2"/>
       <c r="M213" s="2"/>
       <c r="N213" s="2"/>
@@ -5276,7 +5274,7 @@
       <c r="H214" s="2"/>
       <c r="I214" s="7"/>
       <c r="J214" s="2"/>
-      <c r="K214" s="2"/>
+      <c r="K214" s="11"/>
       <c r="L214" s="2"/>
       <c r="M214" s="2"/>
       <c r="N214" s="2"/>
@@ -5296,7 +5294,7 @@
       <c r="H215" s="2"/>
       <c r="I215" s="7"/>
       <c r="J215" s="2"/>
-      <c r="K215" s="2"/>
+      <c r="K215" s="11"/>
       <c r="L215" s="2"/>
       <c r="M215" s="2"/>
       <c r="N215" s="2"/>
@@ -5316,7 +5314,7 @@
       <c r="H216" s="2"/>
       <c r="I216" s="7"/>
       <c r="J216" s="2"/>
-      <c r="K216" s="2"/>
+      <c r="K216" s="11"/>
       <c r="L216" s="2"/>
       <c r="M216" s="2"/>
       <c r="N216" s="2"/>
@@ -5336,7 +5334,7 @@
       <c r="H217" s="2"/>
       <c r="I217" s="7"/>
       <c r="J217" s="2"/>
-      <c r="K217" s="2"/>
+      <c r="K217" s="11"/>
       <c r="L217" s="2"/>
       <c r="M217" s="2"/>
       <c r="N217" s="2"/>
@@ -5356,7 +5354,7 @@
       <c r="H218" s="2"/>
       <c r="I218" s="7"/>
       <c r="J218" s="2"/>
-      <c r="K218" s="2"/>
+      <c r="K218" s="11"/>
       <c r="L218" s="2"/>
       <c r="M218" s="2"/>
       <c r="N218" s="2"/>
@@ -5376,7 +5374,7 @@
       <c r="H219" s="2"/>
       <c r="I219" s="7"/>
       <c r="J219" s="2"/>
-      <c r="K219" s="2"/>
+      <c r="K219" s="11"/>
       <c r="L219" s="2"/>
       <c r="M219" s="2"/>
       <c r="N219" s="2"/>
@@ -5396,7 +5394,7 @@
       <c r="H220" s="2"/>
       <c r="I220" s="7"/>
       <c r="J220" s="2"/>
-      <c r="K220" s="2"/>
+      <c r="K220" s="11"/>
       <c r="L220" s="2"/>
       <c r="M220" s="2"/>
       <c r="N220" s="2"/>
@@ -5416,7 +5414,7 @@
       <c r="H221" s="2"/>
       <c r="I221" s="7"/>
       <c r="J221" s="2"/>
-      <c r="K221" s="2"/>
+      <c r="K221" s="11"/>
       <c r="L221" s="2"/>
       <c r="M221" s="2"/>
       <c r="N221" s="2"/>
@@ -5436,7 +5434,7 @@
       <c r="H222" s="2"/>
       <c r="I222" s="7"/>
       <c r="J222" s="2"/>
-      <c r="K222" s="2"/>
+      <c r="K222" s="11"/>
       <c r="L222" s="2"/>
       <c r="M222" s="2"/>
       <c r="N222" s="2"/>
@@ -5456,7 +5454,7 @@
       <c r="H223" s="2"/>
       <c r="I223" s="7"/>
       <c r="J223" s="2"/>
-      <c r="K223" s="2"/>
+      <c r="K223" s="11"/>
       <c r="L223" s="2"/>
       <c r="M223" s="2"/>
       <c r="N223" s="2"/>
@@ -5476,7 +5474,7 @@
       <c r="H224" s="2"/>
       <c r="I224" s="7"/>
       <c r="J224" s="2"/>
-      <c r="K224" s="2"/>
+      <c r="K224" s="11"/>
       <c r="L224" s="2"/>
       <c r="M224" s="2"/>
       <c r="N224" s="2"/>
@@ -5496,7 +5494,7 @@
       <c r="H225" s="2"/>
       <c r="I225" s="7"/>
       <c r="J225" s="2"/>
-      <c r="K225" s="2"/>
+      <c r="K225" s="11"/>
       <c r="L225" s="2"/>
       <c r="M225" s="2"/>
       <c r="N225" s="2"/>
@@ -5516,7 +5514,7 @@
       <c r="H226" s="2"/>
       <c r="I226" s="7"/>
       <c r="J226" s="2"/>
-      <c r="K226" s="2"/>
+      <c r="K226" s="11"/>
       <c r="L226" s="2"/>
       <c r="M226" s="2"/>
       <c r="N226" s="2"/>
@@ -5536,7 +5534,7 @@
       <c r="H227" s="2"/>
       <c r="I227" s="7"/>
       <c r="J227" s="2"/>
-      <c r="K227" s="2"/>
+      <c r="K227" s="11"/>
       <c r="L227" s="2"/>
       <c r="M227" s="2"/>
       <c r="N227" s="2"/>
@@ -5556,7 +5554,7 @@
       <c r="H228" s="2"/>
       <c r="I228" s="7"/>
       <c r="J228" s="2"/>
-      <c r="K228" s="2"/>
+      <c r="K228" s="11"/>
       <c r="L228" s="2"/>
       <c r="M228" s="2"/>
       <c r="N228" s="2"/>
@@ -5576,7 +5574,7 @@
       <c r="H229" s="2"/>
       <c r="I229" s="7"/>
       <c r="J229" s="2"/>
-      <c r="K229" s="2"/>
+      <c r="K229" s="11"/>
       <c r="L229" s="2"/>
       <c r="M229" s="2"/>
       <c r="N229" s="2"/>
@@ -5596,7 +5594,7 @@
       <c r="H230" s="2"/>
       <c r="I230" s="7"/>
       <c r="J230" s="2"/>
-      <c r="K230" s="2"/>
+      <c r="K230" s="11"/>
       <c r="L230" s="2"/>
       <c r="M230" s="2"/>
       <c r="N230" s="2"/>
@@ -5616,7 +5614,7 @@
       <c r="H231" s="2"/>
       <c r="I231" s="7"/>
       <c r="J231" s="2"/>
-      <c r="K231" s="2"/>
+      <c r="K231" s="11"/>
       <c r="L231" s="2"/>
       <c r="M231" s="2"/>
       <c r="N231" s="2"/>
@@ -5636,7 +5634,7 @@
       <c r="H232" s="2"/>
       <c r="I232" s="7"/>
       <c r="J232" s="2"/>
-      <c r="K232" s="2"/>
+      <c r="K232" s="11"/>
       <c r="L232" s="2"/>
       <c r="M232" s="2"/>
       <c r="N232" s="2"/>
@@ -5656,7 +5654,7 @@
       <c r="H233" s="2"/>
       <c r="I233" s="7"/>
       <c r="J233" s="2"/>
-      <c r="K233" s="2"/>
+      <c r="K233" s="11"/>
       <c r="L233" s="2"/>
       <c r="M233" s="2"/>
       <c r="N233" s="2"/>
@@ -5676,7 +5674,7 @@
       <c r="H234" s="2"/>
       <c r="I234" s="7"/>
       <c r="J234" s="2"/>
-      <c r="K234" s="2"/>
+      <c r="K234" s="11"/>
       <c r="L234" s="2"/>
       <c r="M234" s="2"/>
       <c r="N234" s="2"/>
@@ -5696,7 +5694,7 @@
       <c r="H235" s="2"/>
       <c r="I235" s="7"/>
       <c r="J235" s="2"/>
-      <c r="K235" s="2"/>
+      <c r="K235" s="11"/>
       <c r="L235" s="2"/>
       <c r="M235" s="2"/>
       <c r="N235" s="2"/>
@@ -5716,7 +5714,7 @@
       <c r="H236" s="2"/>
       <c r="I236" s="7"/>
       <c r="J236" s="2"/>
-      <c r="K236" s="2"/>
+      <c r="K236" s="11"/>
       <c r="L236" s="2"/>
       <c r="M236" s="2"/>
       <c r="N236" s="2"/>
@@ -5736,7 +5734,7 @@
       <c r="H237" s="2"/>
       <c r="I237" s="7"/>
       <c r="J237" s="2"/>
-      <c r="K237" s="2"/>
+      <c r="K237" s="11"/>
       <c r="L237" s="2"/>
       <c r="M237" s="2"/>
       <c r="N237" s="2"/>
@@ -5756,7 +5754,7 @@
       <c r="H238" s="2"/>
       <c r="I238" s="7"/>
       <c r="J238" s="2"/>
-      <c r="K238" s="2"/>
+      <c r="K238" s="11"/>
       <c r="L238" s="2"/>
       <c r="M238" s="2"/>
       <c r="N238" s="2"/>
@@ -5776,7 +5774,7 @@
       <c r="H239" s="2"/>
       <c r="I239" s="7"/>
       <c r="J239" s="2"/>
-      <c r="K239" s="2"/>
+      <c r="K239" s="11"/>
       <c r="L239" s="2"/>
       <c r="M239" s="2"/>
       <c r="N239" s="2"/>
@@ -5796,7 +5794,7 @@
       <c r="H240" s="2"/>
       <c r="I240" s="7"/>
       <c r="J240" s="2"/>
-      <c r="K240" s="2"/>
+      <c r="K240" s="11"/>
       <c r="L240" s="2"/>
       <c r="M240" s="2"/>
       <c r="N240" s="2"/>
@@ -5816,7 +5814,7 @@
       <c r="H241" s="2"/>
       <c r="I241" s="7"/>
       <c r="J241" s="2"/>
-      <c r="K241" s="2"/>
+      <c r="K241" s="11"/>
       <c r="L241" s="2"/>
       <c r="M241" s="2"/>
       <c r="N241" s="2"/>
@@ -5836,7 +5834,7 @@
       <c r="H242" s="2"/>
       <c r="I242" s="7"/>
       <c r="J242" s="2"/>
-      <c r="K242" s="2"/>
+      <c r="K242" s="11"/>
       <c r="L242" s="2"/>
       <c r="M242" s="2"/>
       <c r="N242" s="2"/>
@@ -5856,7 +5854,7 @@
       <c r="H243" s="2"/>
       <c r="I243" s="7"/>
       <c r="J243" s="2"/>
-      <c r="K243" s="2"/>
+      <c r="K243" s="11"/>
       <c r="L243" s="2"/>
       <c r="M243" s="2"/>
       <c r="N243" s="2"/>
@@ -5876,7 +5874,7 @@
       <c r="H244" s="2"/>
       <c r="I244" s="7"/>
       <c r="J244" s="2"/>
-      <c r="K244" s="2"/>
+      <c r="K244" s="11"/>
       <c r="L244" s="2"/>
       <c r="M244" s="2"/>
       <c r="N244" s="2"/>
@@ -5896,7 +5894,7 @@
       <c r="H245" s="2"/>
       <c r="I245" s="7"/>
       <c r="J245" s="2"/>
-      <c r="K245" s="2"/>
+      <c r="K245" s="11"/>
       <c r="L245" s="2"/>
       <c r="M245" s="2"/>
       <c r="N245" s="2"/>
@@ -5916,7 +5914,7 @@
       <c r="H246" s="2"/>
       <c r="I246" s="7"/>
       <c r="J246" s="2"/>
-      <c r="K246" s="2"/>
+      <c r="K246" s="11"/>
       <c r="L246" s="2"/>
       <c r="M246" s="2"/>
       <c r="N246" s="2"/>
@@ -5936,7 +5934,7 @@
       <c r="H247" s="2"/>
       <c r="I247" s="7"/>
       <c r="J247" s="2"/>
-      <c r="K247" s="2"/>
+      <c r="K247" s="11"/>
       <c r="L247" s="2"/>
       <c r="M247" s="2"/>
       <c r="N247" s="2"/>
@@ -5956,7 +5954,7 @@
       <c r="H248" s="2"/>
       <c r="I248" s="7"/>
       <c r="J248" s="2"/>
-      <c r="K248" s="2"/>
+      <c r="K248" s="11"/>
       <c r="L248" s="2"/>
       <c r="M248" s="2"/>
       <c r="N248" s="2"/>
@@ -5976,7 +5974,7 @@
       <c r="H249" s="2"/>
       <c r="I249" s="7"/>
       <c r="J249" s="2"/>
-      <c r="K249" s="2"/>
+      <c r="K249" s="11"/>
       <c r="L249" s="2"/>
       <c r="M249" s="2"/>
       <c r="N249" s="2"/>
@@ -5996,7 +5994,7 @@
       <c r="H250" s="2"/>
       <c r="I250" s="7"/>
       <c r="J250" s="2"/>
-      <c r="K250" s="2"/>
+      <c r="K250" s="11"/>
       <c r="L250" s="2"/>
       <c r="M250" s="2"/>
       <c r="N250" s="2"/>
@@ -6016,7 +6014,7 @@
       <c r="H251" s="2"/>
       <c r="I251" s="7"/>
       <c r="J251" s="2"/>
-      <c r="K251" s="2"/>
+      <c r="K251" s="11"/>
       <c r="L251" s="2"/>
       <c r="M251" s="2"/>
       <c r="N251" s="2"/>
@@ -6036,7 +6034,7 @@
       <c r="H252" s="2"/>
       <c r="I252" s="7"/>
       <c r="J252" s="2"/>
-      <c r="K252" s="2"/>
+      <c r="K252" s="11"/>
       <c r="L252" s="2"/>
       <c r="M252" s="2"/>
       <c r="N252" s="2"/>
@@ -6056,7 +6054,7 @@
       <c r="H253" s="2"/>
       <c r="I253" s="7"/>
       <c r="J253" s="2"/>
-      <c r="K253" s="2"/>
+      <c r="K253" s="11"/>
       <c r="L253" s="2"/>
       <c r="M253" s="2"/>
       <c r="N253" s="2"/>
@@ -6076,7 +6074,7 @@
       <c r="H254" s="2"/>
       <c r="I254" s="7"/>
       <c r="J254" s="2"/>
-      <c r="K254" s="2"/>
+      <c r="K254" s="11"/>
       <c r="L254" s="2"/>
       <c r="M254" s="2"/>
       <c r="N254" s="2"/>
@@ -6096,7 +6094,7 @@
       <c r="H255" s="2"/>
       <c r="I255" s="7"/>
       <c r="J255" s="2"/>
-      <c r="K255" s="2"/>
+      <c r="K255" s="11"/>
       <c r="L255" s="2"/>
       <c r="M255" s="2"/>
       <c r="N255" s="2"/>
@@ -6116,7 +6114,7 @@
       <c r="H256" s="2"/>
       <c r="I256" s="7"/>
       <c r="J256" s="2"/>
-      <c r="K256" s="2"/>
+      <c r="K256" s="11"/>
       <c r="L256" s="2"/>
       <c r="M256" s="2"/>
       <c r="N256" s="2"/>
@@ -6136,7 +6134,7 @@
       <c r="H257" s="2"/>
       <c r="I257" s="7"/>
       <c r="J257" s="2"/>
-      <c r="K257" s="2"/>
+      <c r="K257" s="11"/>
       <c r="L257" s="2"/>
       <c r="M257" s="2"/>
       <c r="N257" s="2"/>
@@ -6156,7 +6154,7 @@
       <c r="H258" s="2"/>
       <c r="I258" s="7"/>
       <c r="J258" s="2"/>
-      <c r="K258" s="2"/>
+      <c r="K258" s="11"/>
       <c r="L258" s="2"/>
       <c r="M258" s="2"/>
       <c r="N258" s="2"/>
@@ -6176,7 +6174,7 @@
       <c r="H259" s="2"/>
       <c r="I259" s="7"/>
       <c r="J259" s="2"/>
-      <c r="K259" s="2"/>
+      <c r="K259" s="11"/>
       <c r="L259" s="2"/>
       <c r="M259" s="2"/>
       <c r="N259" s="2"/>
@@ -6196,7 +6194,7 @@
       <c r="H260" s="2"/>
       <c r="I260" s="7"/>
       <c r="J260" s="2"/>
-      <c r="K260" s="2"/>
+      <c r="K260" s="11"/>
       <c r="L260" s="2"/>
       <c r="M260" s="2"/>
       <c r="N260" s="2"/>
@@ -6216,7 +6214,7 @@
       <c r="H261" s="2"/>
       <c r="I261" s="7"/>
       <c r="J261" s="2"/>
-      <c r="K261" s="2"/>
+      <c r="K261" s="11"/>
       <c r="L261" s="2"/>
       <c r="M261" s="2"/>
       <c r="N261" s="2"/>
@@ -6236,7 +6234,7 @@
       <c r="H262" s="2"/>
       <c r="I262" s="7"/>
       <c r="J262" s="2"/>
-      <c r="K262" s="2"/>
+      <c r="K262" s="11"/>
       <c r="L262" s="2"/>
       <c r="M262" s="2"/>
       <c r="N262" s="2"/>
@@ -6256,7 +6254,7 @@
       <c r="H263" s="2"/>
       <c r="I263" s="7"/>
       <c r="J263" s="2"/>
-      <c r="K263" s="2"/>
+      <c r="K263" s="11"/>
       <c r="L263" s="2"/>
       <c r="M263" s="2"/>
       <c r="N263" s="2"/>
@@ -6276,7 +6274,7 @@
       <c r="H264" s="2"/>
       <c r="I264" s="7"/>
       <c r="J264" s="2"/>
-      <c r="K264" s="2"/>
+      <c r="K264" s="11"/>
       <c r="L264" s="2"/>
       <c r="M264" s="2"/>
       <c r="N264" s="2"/>
@@ -6296,7 +6294,7 @@
       <c r="H265" s="2"/>
       <c r="I265" s="7"/>
       <c r="J265" s="2"/>
-      <c r="K265" s="2"/>
+      <c r="K265" s="11"/>
       <c r="L265" s="2"/>
       <c r="M265" s="2"/>
       <c r="N265" s="2"/>
@@ -6316,7 +6314,7 @@
       <c r="H266" s="2"/>
       <c r="I266" s="7"/>
       <c r="J266" s="2"/>
-      <c r="K266" s="2"/>
+      <c r="K266" s="11"/>
       <c r="L266" s="2"/>
       <c r="M266" s="2"/>
       <c r="N266" s="2"/>
@@ -6336,7 +6334,7 @@
       <c r="H267" s="2"/>
       <c r="I267" s="7"/>
       <c r="J267" s="2"/>
-      <c r="K267" s="2"/>
+      <c r="K267" s="11"/>
       <c r="L267" s="2"/>
       <c r="M267" s="2"/>
       <c r="N267" s="2"/>
@@ -6356,7 +6354,7 @@
       <c r="H268" s="2"/>
       <c r="I268" s="7"/>
       <c r="J268" s="2"/>
-      <c r="K268" s="2"/>
+      <c r="K268" s="11"/>
       <c r="L268" s="2"/>
       <c r="M268" s="2"/>
       <c r="N268" s="2"/>
@@ -6376,7 +6374,7 @@
       <c r="H269" s="2"/>
       <c r="I269" s="7"/>
       <c r="J269" s="2"/>
-      <c r="K269" s="2"/>
+      <c r="K269" s="11"/>
       <c r="L269" s="2"/>
       <c r="M269" s="2"/>
       <c r="N269" s="2"/>
@@ -6396,7 +6394,7 @@
       <c r="H270" s="2"/>
       <c r="I270" s="7"/>
       <c r="J270" s="2"/>
-      <c r="K270" s="2"/>
+      <c r="K270" s="11"/>
       <c r="L270" s="2"/>
       <c r="M270" s="2"/>
       <c r="N270" s="2"/>
@@ -6416,7 +6414,7 @@
       <c r="H271" s="2"/>
       <c r="I271" s="7"/>
       <c r="J271" s="2"/>
-      <c r="K271" s="2"/>
+      <c r="K271" s="11"/>
       <c r="L271" s="2"/>
       <c r="M271" s="2"/>
       <c r="N271" s="2"/>
@@ -6436,7 +6434,7 @@
       <c r="H272" s="2"/>
       <c r="I272" s="7"/>
       <c r="J272" s="2"/>
-      <c r="K272" s="2"/>
+      <c r="K272" s="11"/>
       <c r="L272" s="2"/>
       <c r="M272" s="2"/>
       <c r="N272" s="2"/>
@@ -6456,7 +6454,7 @@
       <c r="H273" s="2"/>
       <c r="I273" s="7"/>
       <c r="J273" s="2"/>
-      <c r="K273" s="2"/>
+      <c r="K273" s="11"/>
       <c r="L273" s="2"/>
       <c r="M273" s="2"/>
       <c r="N273" s="2"/>
@@ -6476,7 +6474,7 @@
       <c r="H274" s="2"/>
       <c r="I274" s="7"/>
       <c r="J274" s="2"/>
-      <c r="K274" s="2"/>
+      <c r="K274" s="11"/>
       <c r="L274" s="2"/>
       <c r="M274" s="2"/>
       <c r="N274" s="2"/>
@@ -6496,7 +6494,7 @@
       <c r="H275" s="2"/>
       <c r="I275" s="7"/>
       <c r="J275" s="2"/>
-      <c r="K275" s="2"/>
+      <c r="K275" s="11"/>
       <c r="L275" s="2"/>
       <c r="M275" s="2"/>
       <c r="N275" s="2"/>
@@ -6516,7 +6514,7 @@
       <c r="H276" s="2"/>
       <c r="I276" s="7"/>
       <c r="J276" s="2"/>
-      <c r="K276" s="2"/>
+      <c r="K276" s="11"/>
       <c r="L276" s="2"/>
       <c r="M276" s="2"/>
       <c r="N276" s="2"/>
@@ -6536,7 +6534,7 @@
       <c r="H277" s="2"/>
       <c r="I277" s="7"/>
       <c r="J277" s="2"/>
-      <c r="K277" s="2"/>
+      <c r="K277" s="11"/>
       <c r="L277" s="2"/>
       <c r="M277" s="2"/>
       <c r="N277" s="2"/>
@@ -6556,7 +6554,7 @@
       <c r="H278" s="2"/>
       <c r="I278" s="7"/>
       <c r="J278" s="2"/>
-      <c r="K278" s="2"/>
+      <c r="K278" s="11"/>
       <c r="L278" s="2"/>
       <c r="M278" s="2"/>
       <c r="N278" s="2"/>
@@ -6576,7 +6574,7 @@
       <c r="H279" s="2"/>
       <c r="I279" s="7"/>
       <c r="J279" s="2"/>
-      <c r="K279" s="2"/>
+      <c r="K279" s="11"/>
       <c r="L279" s="2"/>
       <c r="M279" s="2"/>
       <c r="N279" s="2"/>
@@ -6596,7 +6594,7 @@
       <c r="H280" s="2"/>
       <c r="I280" s="7"/>
       <c r="J280" s="2"/>
-      <c r="K280" s="2"/>
+      <c r="K280" s="11"/>
       <c r="L280" s="2"/>
       <c r="M280" s="2"/>
       <c r="N280" s="2"/>
@@ -6616,7 +6614,7 @@
       <c r="H281" s="2"/>
       <c r="I281" s="7"/>
       <c r="J281" s="2"/>
-      <c r="K281" s="2"/>
+      <c r="K281" s="11"/>
       <c r="L281" s="2"/>
       <c r="M281" s="2"/>
       <c r="N281" s="2"/>
@@ -6636,7 +6634,7 @@
       <c r="H282" s="2"/>
       <c r="I282" s="7"/>
       <c r="J282" s="2"/>
-      <c r="K282" s="2"/>
+      <c r="K282" s="11"/>
       <c r="L282" s="2"/>
       <c r="M282" s="2"/>
       <c r="N282" s="2"/>
@@ -6656,7 +6654,7 @@
       <c r="H283" s="2"/>
       <c r="I283" s="7"/>
       <c r="J283" s="2"/>
-      <c r="K283" s="2"/>
+      <c r="K283" s="11"/>
       <c r="L283" s="2"/>
       <c r="M283" s="2"/>
       <c r="N283" s="2"/>
@@ -6676,7 +6674,7 @@
       <c r="H284" s="2"/>
       <c r="I284" s="7"/>
       <c r="J284" s="2"/>
-      <c r="K284" s="2"/>
+      <c r="K284" s="11"/>
       <c r="L284" s="2"/>
       <c r="M284" s="2"/>
       <c r="N284" s="2"/>
@@ -6696,7 +6694,7 @@
       <c r="H285" s="2"/>
       <c r="I285" s="7"/>
       <c r="J285" s="2"/>
-      <c r="K285" s="2"/>
+      <c r="K285" s="11"/>
       <c r="L285" s="2"/>
       <c r="M285" s="2"/>
       <c r="N285" s="2"/>
@@ -6716,7 +6714,7 @@
       <c r="H286" s="2"/>
       <c r="I286" s="7"/>
       <c r="J286" s="2"/>
-      <c r="K286" s="2"/>
+      <c r="K286" s="11"/>
       <c r="L286" s="2"/>
       <c r="M286" s="2"/>
       <c r="N286" s="2"/>
@@ -6736,7 +6734,7 @@
       <c r="H287" s="2"/>
       <c r="I287" s="7"/>
       <c r="J287" s="2"/>
-      <c r="K287" s="2"/>
+      <c r="K287" s="11"/>
       <c r="L287" s="2"/>
       <c r="M287" s="2"/>
       <c r="N287" s="2"/>
@@ -6756,7 +6754,7 @@
       <c r="H288" s="2"/>
       <c r="I288" s="7"/>
       <c r="J288" s="2"/>
-      <c r="K288" s="2"/>
+      <c r="K288" s="11"/>
       <c r="L288" s="2"/>
       <c r="M288" s="2"/>
       <c r="N288" s="2"/>
@@ -6776,7 +6774,7 @@
       <c r="H289" s="2"/>
       <c r="I289" s="7"/>
       <c r="J289" s="2"/>
-      <c r="K289" s="2"/>
+      <c r="K289" s="11"/>
       <c r="L289" s="2"/>
       <c r="M289" s="2"/>
       <c r="N289" s="2"/>
@@ -6796,7 +6794,7 @@
       <c r="H290" s="2"/>
       <c r="I290" s="7"/>
       <c r="J290" s="2"/>
-      <c r="K290" s="2"/>
+      <c r="K290" s="11"/>
       <c r="L290" s="2"/>
       <c r="M290" s="2"/>
       <c r="N290" s="2"/>
@@ -6816,7 +6814,7 @@
       <c r="H291" s="2"/>
       <c r="I291" s="7"/>
       <c r="J291" s="2"/>
-      <c r="K291" s="2"/>
+      <c r="K291" s="11"/>
       <c r="L291" s="2"/>
       <c r="M291" s="2"/>
       <c r="N291" s="2"/>
@@ -6836,7 +6834,7 @@
       <c r="H292" s="2"/>
       <c r="I292" s="7"/>
       <c r="J292" s="2"/>
-      <c r="K292" s="2"/>
+      <c r="K292" s="11"/>
       <c r="L292" s="2"/>
       <c r="M292" s="2"/>
       <c r="N292" s="2"/>
@@ -6856,7 +6854,7 @@
       <c r="H293" s="2"/>
       <c r="I293" s="7"/>
       <c r="J293" s="2"/>
-      <c r="K293" s="2"/>
+      <c r="K293" s="11"/>
       <c r="L293" s="2"/>
       <c r="M293" s="2"/>
       <c r="N293" s="2"/>
@@ -6876,7 +6874,7 @@
       <c r="H294" s="2"/>
       <c r="I294" s="7"/>
       <c r="J294" s="2"/>
-      <c r="K294" s="2"/>
+      <c r="K294" s="11"/>
       <c r="L294" s="2"/>
       <c r="M294" s="2"/>
       <c r="N294" s="2"/>
@@ -6896,7 +6894,7 @@
       <c r="H295" s="2"/>
       <c r="I295" s="7"/>
       <c r="J295" s="2"/>
-      <c r="K295" s="2"/>
+      <c r="K295" s="11"/>
       <c r="L295" s="2"/>
       <c r="M295" s="2"/>
       <c r="N295" s="2"/>
@@ -6916,7 +6914,7 @@
       <c r="H296" s="2"/>
       <c r="I296" s="7"/>
       <c r="J296" s="2"/>
-      <c r="K296" s="2"/>
+      <c r="K296" s="11"/>
       <c r="L296" s="2"/>
       <c r="M296" s="2"/>
       <c r="N296" s="2"/>
@@ -6936,7 +6934,7 @@
       <c r="H297" s="2"/>
       <c r="I297" s="7"/>
       <c r="J297" s="2"/>
-      <c r="K297" s="2"/>
+      <c r="K297" s="11"/>
       <c r="L297" s="2"/>
       <c r="M297" s="2"/>
       <c r="N297" s="2"/>
@@ -6956,7 +6954,7 @@
       <c r="H298" s="2"/>
       <c r="I298" s="7"/>
       <c r="J298" s="2"/>
-      <c r="K298" s="2"/>
+      <c r="K298" s="11"/>
       <c r="L298" s="2"/>
       <c r="M298" s="2"/>
       <c r="N298" s="2"/>
@@ -6976,7 +6974,7 @@
       <c r="H299" s="2"/>
       <c r="I299" s="7"/>
       <c r="J299" s="2"/>
-      <c r="K299" s="2"/>
+      <c r="K299" s="11"/>
       <c r="L299" s="2"/>
       <c r="M299" s="2"/>
       <c r="N299" s="2"/>
@@ -6996,7 +6994,7 @@
       <c r="H300" s="2"/>
       <c r="I300" s="7"/>
       <c r="J300" s="2"/>
-      <c r="K300" s="2"/>
+      <c r="K300" s="11"/>
       <c r="L300" s="2"/>
       <c r="M300" s="2"/>
       <c r="N300" s="2"/>
@@ -7016,7 +7014,7 @@
       <c r="H301" s="2"/>
       <c r="I301" s="7"/>
       <c r="J301" s="2"/>
-      <c r="K301" s="2"/>
+      <c r="K301" s="11"/>
       <c r="L301" s="2"/>
       <c r="M301" s="2"/>
       <c r="N301" s="2"/>
@@ -7036,7 +7034,7 @@
       <c r="H302" s="2"/>
       <c r="I302" s="7"/>
       <c r="J302" s="2"/>
-      <c r="K302" s="2"/>
+      <c r="K302" s="11"/>
       <c r="L302" s="2"/>
       <c r="M302" s="2"/>
       <c r="N302" s="2"/>
@@ -7056,7 +7054,7 @@
       <c r="H303" s="2"/>
       <c r="I303" s="7"/>
       <c r="J303" s="2"/>
-      <c r="K303" s="2"/>
+      <c r="K303" s="11"/>
       <c r="L303" s="2"/>
       <c r="M303" s="2"/>
       <c r="N303" s="2"/>
@@ -7076,7 +7074,7 @@
       <c r="H304" s="2"/>
       <c r="I304" s="7"/>
       <c r="J304" s="2"/>
-      <c r="K304" s="2"/>
+      <c r="K304" s="11"/>
       <c r="L304" s="2"/>
       <c r="M304" s="2"/>
       <c r="N304" s="2"/>
@@ -7096,7 +7094,7 @@
       <c r="H305" s="2"/>
       <c r="I305" s="7"/>
       <c r="J305" s="2"/>
-      <c r="K305" s="2"/>
+      <c r="K305" s="11"/>
       <c r="L305" s="2"/>
       <c r="M305" s="2"/>
       <c r="N305" s="2"/>
@@ -7116,7 +7114,7 @@
       <c r="H306" s="2"/>
       <c r="I306" s="7"/>
       <c r="J306" s="2"/>
-      <c r="K306" s="2"/>
+      <c r="K306" s="11"/>
       <c r="L306" s="2"/>
       <c r="M306" s="2"/>
       <c r="N306" s="2"/>
@@ -7136,7 +7134,7 @@
       <c r="H307" s="2"/>
       <c r="I307" s="7"/>
       <c r="J307" s="2"/>
-      <c r="K307" s="2"/>
+      <c r="K307" s="11"/>
       <c r="L307" s="2"/>
       <c r="M307" s="2"/>
       <c r="N307" s="2"/>
@@ -7156,7 +7154,7 @@
       <c r="H308" s="2"/>
       <c r="I308" s="7"/>
       <c r="J308" s="2"/>
-      <c r="K308" s="2"/>
+      <c r="K308" s="11"/>
       <c r="L308" s="2"/>
       <c r="M308" s="2"/>
       <c r="N308" s="2"/>
@@ -7176,7 +7174,7 @@
       <c r="H309" s="2"/>
       <c r="I309" s="7"/>
       <c r="J309" s="2"/>
-      <c r="K309" s="2"/>
+      <c r="K309" s="11"/>
       <c r="L309" s="2"/>
       <c r="M309" s="2"/>
       <c r="N309" s="2"/>
@@ -7196,7 +7194,7 @@
       <c r="H310" s="2"/>
       <c r="I310" s="7"/>
       <c r="J310" s="2"/>
-      <c r="K310" s="2"/>
+      <c r="K310" s="11"/>
       <c r="L310" s="2"/>
       <c r="M310" s="2"/>
       <c r="N310" s="2"/>
@@ -7216,7 +7214,7 @@
       <c r="H311" s="2"/>
       <c r="I311" s="7"/>
       <c r="J311" s="2"/>
-      <c r="K311" s="2"/>
+      <c r="K311" s="11"/>
       <c r="L311" s="2"/>
       <c r="M311" s="2"/>
       <c r="N311" s="2"/>
@@ -7236,7 +7234,7 @@
       <c r="H312" s="2"/>
       <c r="I312" s="7"/>
       <c r="J312" s="2"/>
-      <c r="K312" s="2"/>
+      <c r="K312" s="11"/>
       <c r="L312" s="2"/>
       <c r="M312" s="2"/>
       <c r="N312" s="2"/>
@@ -7256,7 +7254,7 @@
       <c r="H313" s="2"/>
       <c r="I313" s="7"/>
       <c r="J313" s="2"/>
-      <c r="K313" s="2"/>
+      <c r="K313" s="11"/>
       <c r="L313" s="2"/>
       <c r="M313" s="2"/>
       <c r="N313" s="2"/>
@@ -7276,7 +7274,7 @@
       <c r="H314" s="2"/>
       <c r="I314" s="7"/>
       <c r="J314" s="2"/>
-      <c r="K314" s="2"/>
+      <c r="K314" s="11"/>
       <c r="L314" s="2"/>
       <c r="M314" s="2"/>
       <c r="N314" s="2"/>
@@ -7296,7 +7294,7 @@
       <c r="H315" s="2"/>
       <c r="I315" s="7"/>
       <c r="J315" s="2"/>
-      <c r="K315" s="2"/>
+      <c r="K315" s="11"/>
       <c r="L315" s="2"/>
       <c r="M315" s="2"/>
       <c r="N315" s="2"/>
@@ -7316,7 +7314,7 @@
       <c r="H316" s="2"/>
       <c r="I316" s="7"/>
       <c r="J316" s="2"/>
-      <c r="K316" s="2"/>
+      <c r="K316" s="11"/>
       <c r="L316" s="2"/>
       <c r="M316" s="2"/>
       <c r="N316" s="2"/>
@@ -7336,7 +7334,7 @@
       <c r="H317" s="2"/>
       <c r="I317" s="7"/>
       <c r="J317" s="2"/>
-      <c r="K317" s="2"/>
+      <c r="K317" s="11"/>
       <c r="L317" s="2"/>
       <c r="M317" s="2"/>
       <c r="N317" s="2"/>
@@ -7356,7 +7354,7 @@
       <c r="H318" s="2"/>
       <c r="I318" s="7"/>
       <c r="J318" s="2"/>
-      <c r="K318" s="2"/>
+      <c r="K318" s="11"/>
       <c r="L318" s="2"/>
       <c r="M318" s="2"/>
       <c r="N318" s="2"/>
@@ -7376,7 +7374,7 @@
       <c r="H319" s="2"/>
       <c r="I319" s="7"/>
       <c r="J319" s="2"/>
-      <c r="K319" s="2"/>
+      <c r="K319" s="11"/>
       <c r="L319" s="2"/>
       <c r="M319" s="2"/>
       <c r="N319" s="2"/>
@@ -7396,7 +7394,7 @@
       <c r="H320" s="2"/>
       <c r="I320" s="7"/>
       <c r="J320" s="2"/>
-      <c r="K320" s="2"/>
+      <c r="K320" s="11"/>
       <c r="L320" s="2"/>
       <c r="M320" s="2"/>
       <c r="N320" s="2"/>
@@ -7416,7 +7414,7 @@
       <c r="H321" s="2"/>
       <c r="I321" s="7"/>
       <c r="J321" s="2"/>
-      <c r="K321" s="2"/>
+      <c r="K321" s="11"/>
       <c r="L321" s="2"/>
       <c r="M321" s="2"/>
       <c r="N321" s="2"/>
@@ -7436,7 +7434,7 @@
       <c r="H322" s="2"/>
       <c r="I322" s="7"/>
       <c r="J322" s="2"/>
-      <c r="K322" s="2"/>
+      <c r="K322" s="11"/>
       <c r="L322" s="2"/>
       <c r="M322" s="2"/>
       <c r="N322" s="2"/>
@@ -7456,7 +7454,7 @@
       <c r="H323" s="2"/>
       <c r="I323" s="7"/>
       <c r="J323" s="2"/>
-      <c r="K323" s="2"/>
+      <c r="K323" s="11"/>
       <c r="L323" s="2"/>
       <c r="M323" s="2"/>
       <c r="N323" s="2"/>
@@ -7476,7 +7474,7 @@
       <c r="H324" s="2"/>
       <c r="I324" s="7"/>
       <c r="J324" s="2"/>
-      <c r="K324" s="2"/>
+      <c r="K324" s="11"/>
       <c r="L324" s="2"/>
       <c r="M324" s="2"/>
       <c r="N324" s="2"/>
@@ -7496,7 +7494,7 @@
       <c r="H325" s="2"/>
       <c r="I325" s="7"/>
       <c r="J325" s="2"/>
-      <c r="K325" s="2"/>
+      <c r="K325" s="11"/>
       <c r="L325" s="2"/>
       <c r="M325" s="2"/>
       <c r="N325" s="2"/>
@@ -7516,7 +7514,7 @@
       <c r="H326" s="2"/>
       <c r="I326" s="7"/>
       <c r="J326" s="2"/>
-      <c r="K326" s="2"/>
+      <c r="K326" s="11"/>
       <c r="L326" s="2"/>
       <c r="M326" s="2"/>
       <c r="N326" s="2"/>
@@ -7536,7 +7534,7 @@
       <c r="H327" s="2"/>
       <c r="I327" s="7"/>
       <c r="J327" s="2"/>
-      <c r="K327" s="2"/>
+      <c r="K327" s="11"/>
       <c r="L327" s="2"/>
       <c r="M327" s="2"/>
       <c r="N327" s="2"/>
@@ -7556,7 +7554,7 @@
       <c r="H328" s="2"/>
       <c r="I328" s="7"/>
       <c r="J328" s="2"/>
-      <c r="K328" s="2"/>
+      <c r="K328" s="11"/>
       <c r="L328" s="2"/>
       <c r="M328" s="2"/>
       <c r="N328" s="2"/>
@@ -7576,7 +7574,7 @@
       <c r="H329" s="2"/>
       <c r="I329" s="7"/>
       <c r="J329" s="2"/>
-      <c r="K329" s="2"/>
+      <c r="K329" s="11"/>
       <c r="L329" s="2"/>
       <c r="M329" s="2"/>
       <c r="N329" s="2"/>
@@ -7596,7 +7594,7 @@
       <c r="H330" s="2"/>
       <c r="I330" s="7"/>
       <c r="J330" s="2"/>
-      <c r="K330" s="2"/>
+      <c r="K330" s="11"/>
       <c r="L330" s="2"/>
       <c r="M330" s="2"/>
       <c r="N330" s="2"/>
@@ -7616,7 +7614,7 @@
       <c r="H331" s="2"/>
       <c r="I331" s="7"/>
       <c r="J331" s="2"/>
-      <c r="K331" s="2"/>
+      <c r="K331" s="11"/>
       <c r="L331" s="2"/>
       <c r="M331" s="2"/>
       <c r="N331" s="2"/>
@@ -7636,7 +7634,7 @@
       <c r="H332" s="2"/>
       <c r="I332" s="7"/>
       <c r="J332" s="2"/>
-      <c r="K332" s="2"/>
+      <c r="K332" s="11"/>
       <c r="L332" s="2"/>
       <c r="M332" s="2"/>
       <c r="N332" s="2"/>
@@ -7656,7 +7654,7 @@
       <c r="H333" s="2"/>
       <c r="I333" s="7"/>
       <c r="J333" s="2"/>
-      <c r="K333" s="2"/>
+      <c r="K333" s="11"/>
       <c r="L333" s="2"/>
       <c r="M333" s="2"/>
       <c r="N333" s="2"/>
@@ -7676,7 +7674,7 @@
       <c r="H334" s="2"/>
       <c r="I334" s="7"/>
       <c r="J334" s="2"/>
-      <c r="K334" s="2"/>
+      <c r="K334" s="11"/>
       <c r="L334" s="2"/>
       <c r="M334" s="2"/>
       <c r="N334" s="2"/>
@@ -7696,7 +7694,7 @@
       <c r="H335" s="2"/>
       <c r="I335" s="7"/>
       <c r="J335" s="2"/>
-      <c r="K335" s="2"/>
+      <c r="K335" s="11"/>
       <c r="L335" s="2"/>
       <c r="M335" s="2"/>
       <c r="N335" s="2"/>
@@ -7716,7 +7714,7 @@
       <c r="H336" s="2"/>
       <c r="I336" s="7"/>
       <c r="J336" s="2"/>
-      <c r="K336" s="2"/>
+      <c r="K336" s="11"/>
       <c r="L336" s="2"/>
       <c r="M336" s="2"/>
       <c r="N336" s="2"/>
@@ -7736,7 +7734,7 @@
       <c r="H337" s="2"/>
       <c r="I337" s="7"/>
       <c r="J337" s="2"/>
-      <c r="K337" s="2"/>
+      <c r="K337" s="11"/>
       <c r="L337" s="2"/>
       <c r="M337" s="2"/>
       <c r="N337" s="2"/>
@@ -7756,7 +7754,7 @@
       <c r="H338" s="2"/>
       <c r="I338" s="7"/>
       <c r="J338" s="2"/>
-      <c r="K338" s="2"/>
+      <c r="K338" s="11"/>
       <c r="L338" s="2"/>
       <c r="M338" s="2"/>
       <c r="N338" s="2"/>
@@ -7776,7 +7774,7 @@
       <c r="H339" s="2"/>
       <c r="I339" s="7"/>
       <c r="J339" s="2"/>
-      <c r="K339" s="2"/>
+      <c r="K339" s="11"/>
       <c r="L339" s="2"/>
       <c r="M339" s="2"/>
       <c r="N339" s="2"/>
@@ -7796,7 +7794,7 @@
       <c r="H340" s="2"/>
       <c r="I340" s="7"/>
       <c r="J340" s="2"/>
-      <c r="K340" s="2"/>
+      <c r="K340" s="11"/>
       <c r="L340" s="2"/>
       <c r="M340" s="2"/>
       <c r="N340" s="2"/>
@@ -7816,7 +7814,7 @@
       <c r="H341" s="2"/>
       <c r="I341" s="7"/>
       <c r="J341" s="2"/>
-      <c r="K341" s="2"/>
+      <c r="K341" s="11"/>
       <c r="L341" s="2"/>
       <c r="M341" s="2"/>
       <c r="N341" s="2"/>
@@ -7836,7 +7834,7 @@
       <c r="H342" s="2"/>
       <c r="I342" s="7"/>
       <c r="J342" s="2"/>
-      <c r="K342" s="2"/>
+      <c r="K342" s="11"/>
       <c r="L342" s="2"/>
       <c r="M342" s="2"/>
       <c r="N342" s="2"/>
@@ -7856,7 +7854,7 @@
       <c r="H343" s="2"/>
       <c r="I343" s="7"/>
       <c r="J343" s="2"/>
-      <c r="K343" s="2"/>
+      <c r="K343" s="11"/>
       <c r="L343" s="2"/>
       <c r="M343" s="2"/>
       <c r="N343" s="2"/>
@@ -7876,7 +7874,7 @@
       <c r="H344" s="2"/>
       <c r="I344" s="7"/>
       <c r="J344" s="2"/>
-      <c r="K344" s="2"/>
+      <c r="K344" s="11"/>
       <c r="L344" s="2"/>
       <c r="M344" s="2"/>
       <c r="N344" s="2"/>
@@ -7896,7 +7894,7 @@
       <c r="H345" s="2"/>
       <c r="I345" s="7"/>
       <c r="J345" s="2"/>
-      <c r="K345" s="2"/>
+      <c r="K345" s="11"/>
       <c r="L345" s="2"/>
       <c r="M345" s="2"/>
       <c r="N345" s="2"/>
@@ -7916,7 +7914,7 @@
       <c r="H346" s="2"/>
       <c r="I346" s="7"/>
       <c r="J346" s="2"/>
-      <c r="K346" s="2"/>
+      <c r="K346" s="11"/>
       <c r="L346" s="2"/>
       <c r="M346" s="2"/>
       <c r="N346" s="2"/>
@@ -7936,7 +7934,7 @@
       <c r="H347" s="2"/>
       <c r="I347" s="7"/>
       <c r="J347" s="2"/>
-      <c r="K347" s="2"/>
+      <c r="K347" s="11"/>
       <c r="L347" s="2"/>
       <c r="M347" s="2"/>
       <c r="N347" s="2"/>
@@ -7956,7 +7954,7 @@
       <c r="H348" s="2"/>
       <c r="I348" s="7"/>
       <c r="J348" s="2"/>
-      <c r="K348" s="2"/>
+      <c r="K348" s="11"/>
       <c r="L348" s="2"/>
       <c r="M348" s="2"/>
       <c r="N348" s="2"/>
@@ -7976,7 +7974,7 @@
       <c r="H349" s="2"/>
       <c r="I349" s="7"/>
       <c r="J349" s="2"/>
-      <c r="K349" s="2"/>
+      <c r="K349" s="11"/>
       <c r="L349" s="2"/>
       <c r="M349" s="2"/>
       <c r="N349" s="2"/>
@@ -7996,7 +7994,7 @@
       <c r="H350" s="2"/>
       <c r="I350" s="7"/>
       <c r="J350" s="2"/>
-      <c r="K350" s="2"/>
+      <c r="K350" s="11"/>
       <c r="L350" s="2"/>
       <c r="M350" s="2"/>
       <c r="N350" s="2"/>
@@ -8016,7 +8014,7 @@
       <c r="H351" s="2"/>
       <c r="I351" s="7"/>
       <c r="J351" s="2"/>
-      <c r="K351" s="2"/>
+      <c r="K351" s="11"/>
       <c r="L351" s="2"/>
       <c r="M351" s="2"/>
       <c r="N351" s="2"/>
@@ -8036,7 +8034,7 @@
       <c r="H352" s="2"/>
       <c r="I352" s="7"/>
       <c r="J352" s="2"/>
-      <c r="K352" s="2"/>
+      <c r="K352" s="11"/>
       <c r="L352" s="2"/>
       <c r="M352" s="2"/>
       <c r="N352" s="2"/>
@@ -8056,7 +8054,7 @@
       <c r="H353" s="2"/>
       <c r="I353" s="7"/>
       <c r="J353" s="2"/>
-      <c r="K353" s="2"/>
+      <c r="K353" s="11"/>
       <c r="L353" s="2"/>
       <c r="M353" s="2"/>
       <c r="N353" s="2"/>
@@ -8076,7 +8074,7 @@
       <c r="H354" s="2"/>
       <c r="I354" s="7"/>
       <c r="J354" s="2"/>
-      <c r="K354" s="2"/>
+      <c r="K354" s="11"/>
       <c r="L354" s="2"/>
       <c r="M354" s="2"/>
       <c r="N354" s="2"/>
@@ -8096,7 +8094,7 @@
       <c r="H355" s="2"/>
       <c r="I355" s="7"/>
       <c r="J355" s="2"/>
-      <c r="K355" s="2"/>
+      <c r="K355" s="11"/>
       <c r="L355" s="2"/>
       <c r="M355" s="2"/>
       <c r="N355" s="2"/>
@@ -8116,7 +8114,7 @@
       <c r="H356" s="2"/>
       <c r="I356" s="7"/>
       <c r="J356" s="2"/>
-      <c r="K356" s="2"/>
+      <c r="K356" s="11"/>
       <c r="L356" s="2"/>
       <c r="M356" s="2"/>
       <c r="N356" s="2"/>
@@ -8136,7 +8134,7 @@
       <c r="H357" s="2"/>
       <c r="I357" s="7"/>
       <c r="J357" s="2"/>
-      <c r="K357" s="2"/>
+      <c r="K357" s="11"/>
       <c r="L357" s="2"/>
       <c r="M357" s="2"/>
       <c r="N357" s="2"/>
@@ -8156,7 +8154,7 @@
       <c r="H358" s="2"/>
       <c r="I358" s="7"/>
       <c r="J358" s="2"/>
-      <c r="K358" s="2"/>
+      <c r="K358" s="11"/>
       <c r="L358" s="2"/>
       <c r="M358" s="2"/>
       <c r="N358" s="2"/>
@@ -8176,7 +8174,7 @@
       <c r="H359" s="2"/>
       <c r="I359" s="7"/>
       <c r="J359" s="2"/>
-      <c r="K359" s="2"/>
+      <c r="K359" s="11"/>
       <c r="L359" s="2"/>
       <c r="M359" s="2"/>
       <c r="N359" s="2"/>
@@ -8196,7 +8194,7 @@
       <c r="H360" s="2"/>
       <c r="I360" s="7"/>
       <c r="J360" s="2"/>
-      <c r="K360" s="2"/>
+      <c r="K360" s="11"/>
       <c r="L360" s="2"/>
       <c r="M360" s="2"/>
       <c r="N360" s="2"/>
@@ -8216,7 +8214,7 @@
       <c r="H361" s="2"/>
       <c r="I361" s="7"/>
       <c r="J361" s="2"/>
-      <c r="K361" s="2"/>
+      <c r="K361" s="11"/>
       <c r="L361" s="2"/>
       <c r="M361" s="2"/>
       <c r="N361" s="2"/>
@@ -8236,7 +8234,7 @@
       <c r="H362" s="2"/>
       <c r="I362" s="7"/>
       <c r="J362" s="2"/>
-      <c r="K362" s="2"/>
+      <c r="K362" s="11"/>
       <c r="L362" s="2"/>
       <c r="M362" s="2"/>
       <c r="N362" s="2"/>
@@ -8256,7 +8254,7 @@
       <c r="H363" s="2"/>
       <c r="I363" s="7"/>
       <c r="J363" s="2"/>
-      <c r="K363" s="2"/>
+      <c r="K363" s="11"/>
       <c r="L363" s="2"/>
       <c r="M363" s="2"/>
       <c r="N363" s="2"/>
@@ -8276,7 +8274,7 @@
       <c r="H364" s="2"/>
       <c r="I364" s="7"/>
       <c r="J364" s="2"/>
-      <c r="K364" s="2"/>
+      <c r="K364" s="11"/>
       <c r="L364" s="2"/>
       <c r="M364" s="2"/>
       <c r="N364" s="2"/>
@@ -8296,7 +8294,7 @@
       <c r="H365" s="2"/>
       <c r="I365" s="7"/>
       <c r="J365" s="2"/>
-      <c r="K365" s="2"/>
+      <c r="K365" s="11"/>
       <c r="L365" s="2"/>
       <c r="M365" s="2"/>
       <c r="N365" s="2"/>
@@ -8316,7 +8314,7 @@
       <c r="H366" s="2"/>
       <c r="I366" s="7"/>
       <c r="J366" s="2"/>
-      <c r="K366" s="2"/>
+      <c r="K366" s="11"/>
       <c r="L366" s="2"/>
       <c r="M366" s="2"/>
       <c r="N366" s="2"/>
@@ -8336,7 +8334,7 @@
       <c r="H367" s="2"/>
       <c r="I367" s="7"/>
       <c r="J367" s="2"/>
-      <c r="K367" s="2"/>
+      <c r="K367" s="11"/>
       <c r="L367" s="2"/>
       <c r="M367" s="2"/>
       <c r="N367" s="2"/>
@@ -8356,7 +8354,7 @@
       <c r="H368" s="2"/>
       <c r="I368" s="7"/>
       <c r="J368" s="2"/>
-      <c r="K368" s="2"/>
+      <c r="K368" s="11"/>
       <c r="L368" s="2"/>
       <c r="M368" s="2"/>
       <c r="N368" s="2"/>
@@ -8376,7 +8374,7 @@
       <c r="H369" s="2"/>
       <c r="I369" s="7"/>
       <c r="J369" s="2"/>
-      <c r="K369" s="2"/>
+      <c r="K369" s="11"/>
       <c r="L369" s="2"/>
       <c r="M369" s="2"/>
       <c r="N369" s="2"/>
@@ -8396,7 +8394,7 @@
       <c r="H370" s="2"/>
       <c r="I370" s="7"/>
       <c r="J370" s="2"/>
-      <c r="K370" s="2"/>
+      <c r="K370" s="11"/>
       <c r="L370" s="2"/>
       <c r="M370" s="2"/>
       <c r="N370" s="2"/>
@@ -8416,7 +8414,7 @@
       <c r="H371" s="2"/>
       <c r="I371" s="7"/>
       <c r="J371" s="2"/>
-      <c r="K371" s="2"/>
+      <c r="K371" s="11"/>
       <c r="L371" s="2"/>
       <c r="M371" s="2"/>
       <c r="N371" s="2"/>
@@ -8436,7 +8434,7 @@
       <c r="H372" s="2"/>
       <c r="I372" s="7"/>
       <c r="J372" s="2"/>
-      <c r="K372" s="2"/>
+      <c r="K372" s="11"/>
       <c r="L372" s="2"/>
       <c r="M372" s="2"/>
       <c r="N372" s="2"/>
@@ -8456,7 +8454,7 @@
       <c r="H373" s="2"/>
       <c r="I373" s="7"/>
       <c r="J373" s="2"/>
-      <c r="K373" s="2"/>
+      <c r="K373" s="11"/>
       <c r="L373" s="2"/>
       <c r="M373" s="2"/>
       <c r="N373" s="2"/>
@@ -8476,7 +8474,7 @@
       <c r="H374" s="2"/>
       <c r="I374" s="7"/>
       <c r="J374" s="2"/>
-      <c r="K374" s="2"/>
+      <c r="K374" s="11"/>
       <c r="L374" s="2"/>
       <c r="M374" s="2"/>
       <c r="N374" s="2"/>
@@ -8496,7 +8494,7 @@
       <c r="H375" s="2"/>
       <c r="I375" s="7"/>
       <c r="J375" s="2"/>
-      <c r="K375" s="2"/>
+      <c r="K375" s="11"/>
       <c r="L375" s="2"/>
       <c r="M375" s="2"/>
       <c r="N375" s="2"/>
@@ -8516,7 +8514,7 @@
       <c r="H376" s="2"/>
       <c r="I376" s="7"/>
       <c r="J376" s="2"/>
-      <c r="K376" s="2"/>
+      <c r="K376" s="11"/>
       <c r="L376" s="2"/>
       <c r="M376" s="2"/>
       <c r="N376" s="2"/>
@@ -8536,7 +8534,7 @@
       <c r="H377" s="2"/>
       <c r="I377" s="7"/>
       <c r="J377" s="2"/>
-      <c r="K377" s="2"/>
+      <c r="K377" s="11"/>
       <c r="L377" s="2"/>
       <c r="M377" s="2"/>
       <c r="N377" s="2"/>
@@ -8556,7 +8554,7 @@
       <c r="H378" s="2"/>
       <c r="I378" s="7"/>
       <c r="J378" s="2"/>
-      <c r="K378" s="2"/>
+      <c r="K378" s="11"/>
       <c r="L378" s="2"/>
       <c r="M378" s="2"/>
       <c r="N378" s="2"/>
@@ -8576,7 +8574,7 @@
       <c r="H379" s="2"/>
       <c r="I379" s="7"/>
       <c r="J379" s="2"/>
-      <c r="K379" s="2"/>
+      <c r="K379" s="11"/>
       <c r="L379" s="2"/>
       <c r="M379" s="2"/>
       <c r="N379" s="2"/>
@@ -8596,7 +8594,7 @@
       <c r="H380" s="2"/>
       <c r="I380" s="7"/>
       <c r="J380" s="2"/>
-      <c r="K380" s="2"/>
+      <c r="K380" s="11"/>
       <c r="L380" s="2"/>
       <c r="M380" s="2"/>
       <c r="N380" s="2"/>
@@ -8616,7 +8614,7 @@
       <c r="H381" s="2"/>
       <c r="I381" s="7"/>
       <c r="J381" s="2"/>
-      <c r="K381" s="2"/>
+      <c r="K381" s="11"/>
       <c r="L381" s="2"/>
       <c r="M381" s="2"/>
       <c r="N381" s="2"/>
@@ -8636,7 +8634,7 @@
       <c r="H382" s="2"/>
       <c r="I382" s="7"/>
       <c r="J382" s="2"/>
-      <c r="K382" s="2"/>
+      <c r="K382" s="11"/>
       <c r="L382" s="2"/>
       <c r="M382" s="2"/>
       <c r="N382" s="2"/>
@@ -8656,7 +8654,7 @@
       <c r="H383" s="2"/>
       <c r="I383" s="7"/>
       <c r="J383" s="2"/>
-      <c r="K383" s="2"/>
+      <c r="K383" s="11"/>
       <c r="L383" s="2"/>
       <c r="M383" s="2"/>
       <c r="N383" s="2"/>
@@ -8676,7 +8674,7 @@
       <c r="H384" s="2"/>
       <c r="I384" s="7"/>
       <c r="J384" s="2"/>
-      <c r="K384" s="2"/>
+      <c r="K384" s="11"/>
       <c r="L384" s="2"/>
       <c r="M384" s="2"/>
       <c r="N384" s="2"/>
@@ -8696,7 +8694,7 @@
       <c r="H385" s="2"/>
       <c r="I385" s="7"/>
       <c r="J385" s="2"/>
-      <c r="K385" s="2"/>
+      <c r="K385" s="11"/>
       <c r="L385" s="2"/>
       <c r="M385" s="2"/>
       <c r="N385" s="2"/>
@@ -8716,7 +8714,7 @@
       <c r="H386" s="2"/>
       <c r="I386" s="7"/>
       <c r="J386" s="2"/>
-      <c r="K386" s="2"/>
+      <c r="K386" s="11"/>
       <c r="L386" s="2"/>
       <c r="M386" s="2"/>
       <c r="N386" s="2"/>
@@ -8736,7 +8734,7 @@
       <c r="H387" s="2"/>
       <c r="I387" s="7"/>
       <c r="J387" s="2"/>
-      <c r="K387" s="2"/>
+      <c r="K387" s="11"/>
       <c r="L387" s="2"/>
       <c r="M387" s="2"/>
       <c r="N387" s="2"/>
@@ -8756,7 +8754,7 @@
       <c r="H388" s="2"/>
       <c r="I388" s="7"/>
       <c r="J388" s="2"/>
-      <c r="K388" s="2"/>
+      <c r="K388" s="11"/>
       <c r="L388" s="2"/>
       <c r="M388" s="2"/>
       <c r="N388" s="2"/>
@@ -8776,7 +8774,7 @@
       <c r="H389" s="2"/>
       <c r="I389" s="7"/>
       <c r="J389" s="2"/>
-      <c r="K389" s="2"/>
+      <c r="K389" s="11"/>
       <c r="L389" s="2"/>
       <c r="M389" s="2"/>
       <c r="N389" s="2"/>
@@ -8796,7 +8794,7 @@
       <c r="H390" s="2"/>
       <c r="I390" s="7"/>
       <c r="J390" s="2"/>
-      <c r="K390" s="2"/>
+      <c r="K390" s="11"/>
       <c r="L390" s="2"/>
       <c r="M390" s="2"/>
       <c r="N390" s="2"/>
@@ -8816,7 +8814,7 @@
       <c r="H391" s="2"/>
       <c r="I391" s="7"/>
       <c r="J391" s="2"/>
-      <c r="K391" s="2"/>
+      <c r="K391" s="11"/>
       <c r="L391" s="2"/>
       <c r="M391" s="2"/>
       <c r="N391" s="2"/>
@@ -8836,7 +8834,7 @@
       <c r="H392" s="2"/>
       <c r="I392" s="7"/>
       <c r="J392" s="2"/>
-      <c r="K392" s="2"/>
+      <c r="K392" s="11"/>
       <c r="L392" s="2"/>
       <c r="M392" s="2"/>
       <c r="N392" s="2"/>
@@ -8856,7 +8854,7 @@
       <c r="H393" s="2"/>
       <c r="I393" s="7"/>
       <c r="J393" s="2"/>
-      <c r="K393" s="2"/>
+      <c r="K393" s="11"/>
       <c r="L393" s="2"/>
       <c r="M393" s="2"/>
       <c r="N393" s="2"/>
@@ -8876,7 +8874,7 @@
       <c r="H394" s="2"/>
       <c r="I394" s="7"/>
       <c r="J394" s="2"/>
-      <c r="K394" s="2"/>
+      <c r="K394" s="11"/>
       <c r="L394" s="2"/>
       <c r="M394" s="2"/>
       <c r="N394" s="2"/>
@@ -8896,7 +8894,7 @@
       <c r="H395" s="2"/>
       <c r="I395" s="7"/>
       <c r="J395" s="2"/>
-      <c r="K395" s="2"/>
+      <c r="K395" s="11"/>
       <c r="L395" s="2"/>
       <c r="M395" s="2"/>
       <c r="N395" s="2"/>
@@ -8916,7 +8914,7 @@
       <c r="H396" s="2"/>
       <c r="I396" s="7"/>
       <c r="J396" s="2"/>
-      <c r="K396" s="2"/>
+      <c r="K396" s="11"/>
       <c r="L396" s="2"/>
       <c r="M396" s="2"/>
       <c r="N396" s="2"/>
@@ -8926,41 +8924,41 @@
       <c r="R396" s="1"/>
     </row>
     <row r="397" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A397" s="2"/>
-      <c r="B397" s="2"/>
-      <c r="C397" s="2"/>
-      <c r="D397" s="2"/>
-      <c r="E397" s="2"/>
-      <c r="F397" s="2"/>
-      <c r="G397" s="2"/>
-      <c r="H397" s="2"/>
-      <c r="I397" s="7"/>
-      <c r="J397" s="2"/>
-      <c r="K397" s="2"/>
-      <c r="L397" s="2"/>
-      <c r="M397" s="2"/>
-      <c r="N397" s="2"/>
-      <c r="O397" s="2"/>
+      <c r="A397" s="1"/>
+      <c r="B397" s="1"/>
+      <c r="C397" s="1"/>
+      <c r="D397" s="1"/>
+      <c r="E397" s="1"/>
+      <c r="F397" s="1"/>
+      <c r="G397" s="1"/>
+      <c r="H397" s="1"/>
+      <c r="I397" s="1"/>
+      <c r="J397" s="1"/>
+      <c r="K397" s="1"/>
+      <c r="L397" s="1"/>
+      <c r="M397" s="1"/>
+      <c r="N397" s="1"/>
+      <c r="O397" s="1"/>
       <c r="P397" s="1"/>
       <c r="Q397" s="1"/>
       <c r="R397" s="1"/>
     </row>
     <row r="398" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A398" s="2"/>
-      <c r="B398" s="2"/>
-      <c r="C398" s="2"/>
-      <c r="D398" s="2"/>
-      <c r="E398" s="2"/>
-      <c r="F398" s="2"/>
-      <c r="G398" s="2"/>
-      <c r="H398" s="2"/>
-      <c r="I398" s="7"/>
-      <c r="J398" s="2"/>
-      <c r="K398" s="2"/>
-      <c r="L398" s="2"/>
-      <c r="M398" s="2"/>
-      <c r="N398" s="2"/>
-      <c r="O398" s="2"/>
+      <c r="A398" s="1"/>
+      <c r="B398" s="1"/>
+      <c r="C398" s="1"/>
+      <c r="D398" s="1"/>
+      <c r="E398" s="1"/>
+      <c r="F398" s="1"/>
+      <c r="G398" s="1"/>
+      <c r="H398" s="1"/>
+      <c r="I398" s="1"/>
+      <c r="J398" s="1"/>
+      <c r="K398" s="1"/>
+      <c r="L398" s="1"/>
+      <c r="M398" s="1"/>
+      <c r="N398" s="1"/>
+      <c r="O398" s="1"/>
       <c r="P398" s="1"/>
       <c r="Q398" s="1"/>
       <c r="R398" s="1"/>
@@ -16148,42 +16146,10 @@
     <row r="758" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A758" s="1"/>
       <c r="B758" s="1"/>
-      <c r="C758" s="1"/>
-      <c r="D758" s="1"/>
-      <c r="E758" s="1"/>
-      <c r="F758" s="1"/>
-      <c r="G758" s="1"/>
-      <c r="H758" s="1"/>
-      <c r="I758" s="1"/>
-      <c r="J758" s="1"/>
-      <c r="K758" s="1"/>
-      <c r="L758" s="1"/>
-      <c r="M758" s="1"/>
-      <c r="N758" s="1"/>
-      <c r="O758" s="1"/>
-      <c r="P758" s="1"/>
-      <c r="Q758" s="1"/>
-      <c r="R758" s="1"/>
     </row>
     <row r="759" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A759" s="1"/>
       <c r="B759" s="1"/>
-      <c r="C759" s="1"/>
-      <c r="D759" s="1"/>
-      <c r="E759" s="1"/>
-      <c r="F759" s="1"/>
-      <c r="G759" s="1"/>
-      <c r="H759" s="1"/>
-      <c r="I759" s="1"/>
-      <c r="J759" s="1"/>
-      <c r="K759" s="1"/>
-      <c r="L759" s="1"/>
-      <c r="M759" s="1"/>
-      <c r="N759" s="1"/>
-      <c r="O759" s="1"/>
-      <c r="P759" s="1"/>
-      <c r="Q759" s="1"/>
-      <c r="R759" s="1"/>
     </row>
     <row r="760" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A760" s="1"/>
@@ -17953,32 +17919,12 @@
       <c r="A1201" s="1"/>
       <c r="B1201" s="1"/>
     </row>
-    <row r="1202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1202" s="1"/>
-      <c r="B1202" s="1"/>
-    </row>
-    <row r="1203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1203" s="1"/>
-      <c r="B1203" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="F2:F3"/>
-  </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G80">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G78">
       <formula1>"Laki-laki,Perempuan"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4:J398">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J396">
       <formula1>"Islam,Kristen,Khatolik,Hindu,Budha"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>